<commit_message>
Fixed some stupid formatting issue i caused...
</commit_message>
<xml_diff>
--- a/ClashOfClans_TechTree/CoC_Spread.xlsx
+++ b/ClashOfClans_TechTree/CoC_Spread.xlsx
@@ -398,7 +398,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="24">
+  <fills count="25">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -530,6 +530,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="3">
     <border>
@@ -579,7 +585,7 @@
     <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="88">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -836,6 +842,33 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="24" borderId="0" xfId="8" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="24" borderId="0" xfId="10" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="24" borderId="0" xfId="12" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="6" fillId="24" borderId="0" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="24" borderId="0" xfId="4" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="24" borderId="0" xfId="5" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="24" borderId="0" xfId="7" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="24" borderId="0" xfId="9" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="24" borderId="0" xfId="11" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1139,9 +1172,9 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AD145"/>
+  <dimension ref="A1:AD146"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A129" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A63" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
@@ -5865,28 +5898,28 @@
       <c r="AD74" s="3"/>
     </row>
     <row r="75" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C75" s="4"/>
-      <c r="D75" s="4"/>
-      <c r="E75" s="4"/>
-      <c r="F75" s="4"/>
-      <c r="G75" s="4"/>
-      <c r="H75" s="4"/>
-      <c r="I75" s="4"/>
-      <c r="J75" s="4"/>
-      <c r="K75" s="4"/>
-      <c r="L75" s="4"/>
-      <c r="M75" s="4"/>
-      <c r="N75" s="4"/>
-      <c r="O75" s="4"/>
-      <c r="P75" s="4"/>
-      <c r="Q75" s="4"/>
-      <c r="R75" s="4"/>
-      <c r="S75" s="4"/>
-      <c r="T75" s="4"/>
-      <c r="U75" s="4"/>
-      <c r="V75" s="4"/>
-      <c r="W75" s="4"/>
-      <c r="X75" s="4"/>
+      <c r="C75" s="88"/>
+      <c r="D75" s="88"/>
+      <c r="E75" s="88"/>
+      <c r="F75" s="88"/>
+      <c r="G75" s="89"/>
+      <c r="H75" s="89"/>
+      <c r="I75" s="90"/>
+      <c r="J75" s="90"/>
+      <c r="K75" s="91"/>
+      <c r="L75" s="91"/>
+      <c r="M75" s="92"/>
+      <c r="N75" s="92"/>
+      <c r="O75" s="93"/>
+      <c r="P75" s="93"/>
+      <c r="Q75" s="94"/>
+      <c r="R75" s="94"/>
+      <c r="S75" s="95"/>
+      <c r="T75" s="95"/>
+      <c r="U75" s="95"/>
+      <c r="V75" s="95"/>
+      <c r="W75" s="96"/>
+      <c r="X75" s="96"/>
       <c r="Y75" s="4"/>
       <c r="Z75" s="4"/>
       <c r="AA75" s="4"/>
@@ -5898,33 +5931,14 @@
       <c r="A76" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B76" t="s">
-        <v>53</v>
-      </c>
-      <c r="C76" s="16">
-        <v>4000</v>
-      </c>
-      <c r="D76" s="16" t="s">
-        <v>62</v>
-      </c>
-      <c r="E76" s="16">
-        <v>20000</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>66</v>
-      </c>
-      <c r="G76" s="13">
-        <v>200000</v>
-      </c>
-      <c r="H76" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="I76" s="9">
-        <v>1500000</v>
-      </c>
-      <c r="J76" s="9" t="s">
-        <v>87</v>
-      </c>
+      <c r="C76" s="4"/>
+      <c r="D76" s="4"/>
+      <c r="E76" s="4"/>
+      <c r="F76" s="4"/>
+      <c r="G76" s="4"/>
+      <c r="H76" s="4"/>
+      <c r="I76" s="4"/>
+      <c r="J76" s="4"/>
       <c r="K76" s="4"/>
       <c r="L76" s="4"/>
       <c r="M76" s="4"/>
@@ -6005,22 +6019,22 @@
       <c r="B78" t="s">
         <v>53</v>
       </c>
-      <c r="C78" s="11">
+      <c r="C78" s="16">
         <v>4000</v>
       </c>
-      <c r="D78" s="11" t="s">
+      <c r="D78" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E78" s="45">
+      <c r="E78" s="16">
         <v>20000</v>
       </c>
-      <c r="F78" s="45" t="s">
+      <c r="F78" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="G78" s="37">
+      <c r="G78" s="13">
         <v>200000</v>
       </c>
-      <c r="H78" s="37" t="s">
+      <c r="H78" s="13" t="s">
         <v>69</v>
       </c>
       <c r="I78" s="9">
@@ -6109,28 +6123,28 @@
       <c r="B80" t="s">
         <v>53</v>
       </c>
-      <c r="C80" s="7">
+      <c r="C80" s="11">
         <v>4000</v>
       </c>
-      <c r="D80" s="7" t="s">
+      <c r="D80" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E80" s="47">
+      <c r="E80" s="45">
         <v>20000</v>
       </c>
-      <c r="F80" s="47" t="s">
+      <c r="F80" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="G80" s="12">
+      <c r="G80" s="37">
         <v>200000</v>
       </c>
-      <c r="H80" s="12" t="s">
+      <c r="H80" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="I80" s="8">
+      <c r="I80" s="9">
         <v>1500000</v>
       </c>
-      <c r="J80" s="8" t="s">
+      <c r="J80" s="9" t="s">
         <v>87</v>
       </c>
       <c r="K80" s="4"/>
@@ -6161,42 +6175,34 @@
       <c r="B81" t="s">
         <v>53</v>
       </c>
-      <c r="C81" s="20">
-        <v>400</v>
-      </c>
-      <c r="D81" s="20" t="s">
+      <c r="C81" s="7">
+        <v>4000</v>
+      </c>
+      <c r="D81" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E81" s="20">
-        <v>1000</v>
-      </c>
-      <c r="F81" s="20" t="s">
-        <v>85</v>
-      </c>
-      <c r="G81" s="16">
-        <v>10000</v>
-      </c>
-      <c r="H81" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="I81" s="13">
-        <v>100000</v>
-      </c>
-      <c r="J81" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="K81" s="11">
-        <v>1000000</v>
-      </c>
-      <c r="L81" s="11" t="s">
+      <c r="E81" s="47">
+        <v>20000</v>
+      </c>
+      <c r="F81" s="47" t="s">
+        <v>66</v>
+      </c>
+      <c r="G81" s="12">
+        <v>200000</v>
+      </c>
+      <c r="H81" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="I81" s="8">
+        <v>1500000</v>
+      </c>
+      <c r="J81" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="M81" s="9">
-        <v>1500000</v>
-      </c>
-      <c r="N81" s="9" t="s">
-        <v>70</v>
-      </c>
+      <c r="K81" s="4"/>
+      <c r="L81" s="4"/>
+      <c r="M81" s="4"/>
+      <c r="N81" s="4"/>
       <c r="O81" s="4"/>
       <c r="P81" s="4"/>
       <c r="Q81" s="4"/>
@@ -6281,16 +6287,16 @@
       <c r="B83" t="s">
         <v>53</v>
       </c>
-      <c r="C83" s="16">
+      <c r="C83" s="20">
         <v>400</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="D83" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="E83" s="51">
+      <c r="E83" s="20">
         <v>1000</v>
       </c>
-      <c r="F83" s="51" t="s">
+      <c r="F83" s="20" t="s">
         <v>85</v>
       </c>
       <c r="G83" s="16">
@@ -6401,22 +6407,22 @@
       <c r="B85" t="s">
         <v>53</v>
       </c>
-      <c r="C85" s="13">
+      <c r="C85" s="16">
         <v>400</v>
       </c>
-      <c r="D85" s="13" t="s">
+      <c r="D85" s="16" t="s">
         <v>62</v>
       </c>
-      <c r="E85" s="31">
+      <c r="E85" s="51">
         <v>1000</v>
       </c>
-      <c r="F85" s="31" t="s">
+      <c r="F85" s="51" t="s">
         <v>85</v>
       </c>
-      <c r="G85" s="44">
+      <c r="G85" s="16">
         <v>10000</v>
       </c>
-      <c r="H85" s="44" t="s">
+      <c r="H85" s="16" t="s">
         <v>68</v>
       </c>
       <c r="I85" s="13">
@@ -6521,34 +6527,42 @@
       <c r="B87" t="s">
         <v>53</v>
       </c>
-      <c r="C87" s="15">
-        <v>12500</v>
-      </c>
-      <c r="D87" s="15" t="s">
+      <c r="C87" s="13">
+        <v>400</v>
+      </c>
+      <c r="D87" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E87" s="15">
-        <v>75000</v>
-      </c>
-      <c r="F87" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="G87" s="11">
-        <v>750000</v>
-      </c>
-      <c r="H87" s="11" t="s">
+      <c r="E87" s="31">
+        <v>1000</v>
+      </c>
+      <c r="F87" s="31" t="s">
+        <v>85</v>
+      </c>
+      <c r="G87" s="44">
+        <v>10000</v>
+      </c>
+      <c r="H87" s="44" t="s">
+        <v>68</v>
+      </c>
+      <c r="I87" s="13">
+        <v>100000</v>
+      </c>
+      <c r="J87" s="13" t="s">
+        <v>88</v>
+      </c>
+      <c r="K87" s="11">
+        <v>1000000</v>
+      </c>
+      <c r="L87" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="I87" s="7">
-        <v>2500000</v>
-      </c>
-      <c r="J87" s="7" t="s">
-        <v>77</v>
-      </c>
-      <c r="K87" s="4"/>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
-      <c r="N87" s="4"/>
+      <c r="M87" s="9">
+        <v>1500000</v>
+      </c>
+      <c r="N87" s="9" t="s">
+        <v>70</v>
+      </c>
       <c r="O87" s="4"/>
       <c r="P87" s="4"/>
       <c r="Q87" s="4"/>
@@ -6573,16 +6587,16 @@
       <c r="B88" t="s">
         <v>53</v>
       </c>
-      <c r="C88" s="13">
+      <c r="C88" s="15">
         <v>12500</v>
       </c>
-      <c r="D88" s="13" t="s">
+      <c r="D88" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="E88" s="17">
+      <c r="E88" s="15">
         <v>75000</v>
       </c>
-      <c r="F88" s="17" t="s">
+      <c r="F88" s="15" t="s">
         <v>63</v>
       </c>
       <c r="G88" s="11">
@@ -6625,16 +6639,16 @@
       <c r="B89" t="s">
         <v>53</v>
       </c>
-      <c r="C89" s="11">
+      <c r="C89" s="13">
         <v>12500</v>
       </c>
-      <c r="D89" s="11" t="s">
+      <c r="D89" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="E89" s="36">
+      <c r="E89" s="17">
         <v>75000</v>
       </c>
-      <c r="F89" s="36" t="s">
+      <c r="F89" s="17" t="s">
         <v>63</v>
       </c>
       <c r="G89" s="11">
@@ -6677,22 +6691,22 @@
       <c r="B90" t="s">
         <v>53</v>
       </c>
-      <c r="C90" s="9">
+      <c r="C90" s="11">
         <v>12500</v>
       </c>
-      <c r="D90" s="9" t="s">
+      <c r="D90" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E90" s="41">
+      <c r="E90" s="36">
         <v>75000</v>
       </c>
-      <c r="F90" s="41" t="s">
+      <c r="F90" s="36" t="s">
         <v>63</v>
       </c>
-      <c r="G90" s="43">
+      <c r="G90" s="11">
         <v>750000</v>
       </c>
-      <c r="H90" s="43" t="s">
+      <c r="H90" s="11" t="s">
         <v>87</v>
       </c>
       <c r="I90" s="7">
@@ -6729,22 +6743,22 @@
       <c r="B91" t="s">
         <v>53</v>
       </c>
-      <c r="C91" s="7">
+      <c r="C91" s="9">
         <v>12500</v>
       </c>
-      <c r="D91" s="7" t="s">
+      <c r="D91" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E91" s="14">
+      <c r="E91" s="41">
         <v>75000</v>
       </c>
-      <c r="F91" s="14" t="s">
+      <c r="F91" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="G91" s="10">
+      <c r="G91" s="43">
         <v>750000</v>
       </c>
-      <c r="H91" s="10" t="s">
+      <c r="H91" s="43" t="s">
         <v>87</v>
       </c>
       <c r="I91" s="7">
@@ -6781,26 +6795,30 @@
       <c r="B92" t="s">
         <v>53</v>
       </c>
-      <c r="C92" s="13">
-        <v>15000</v>
-      </c>
-      <c r="D92" s="13" t="s">
+      <c r="C92" s="7">
+        <v>12500</v>
+      </c>
+      <c r="D92" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E92" s="9">
-        <v>2000000</v>
-      </c>
-      <c r="F92" s="9" t="s">
+      <c r="E92" s="14">
+        <v>75000</v>
+      </c>
+      <c r="F92" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="G92" s="10">
+        <v>750000</v>
+      </c>
+      <c r="H92" s="10" t="s">
         <v>87</v>
       </c>
-      <c r="G92" s="7">
-        <v>4000000</v>
-      </c>
-      <c r="H92" s="7" t="s">
+      <c r="I92" s="7">
+        <v>2500000</v>
+      </c>
+      <c r="J92" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="I92" s="4"/>
-      <c r="J92" s="4"/>
       <c r="K92" s="4"/>
       <c r="L92" s="4"/>
       <c r="M92" s="4"/>
@@ -6829,10 +6847,10 @@
       <c r="B93" t="s">
         <v>53</v>
       </c>
-      <c r="C93" s="11">
+      <c r="C93" s="13">
         <v>15000</v>
       </c>
-      <c r="D93" s="11" t="s">
+      <c r="D93" s="13" t="s">
         <v>62</v>
       </c>
       <c r="E93" s="9">
@@ -6877,10 +6895,10 @@
       <c r="B94" t="s">
         <v>53</v>
       </c>
-      <c r="C94" s="9">
+      <c r="C94" s="11">
         <v>15000</v>
       </c>
-      <c r="D94" s="9" t="s">
+      <c r="D94" s="11" t="s">
         <v>62</v>
       </c>
       <c r="E94" s="9">
@@ -6973,16 +6991,16 @@
       <c r="B96" t="s">
         <v>53</v>
       </c>
-      <c r="C96" s="7">
+      <c r="C96" s="9">
         <v>15000</v>
       </c>
-      <c r="D96" s="7" t="s">
+      <c r="D96" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="E96" s="8">
+      <c r="E96" s="9">
         <v>2000000</v>
       </c>
-      <c r="F96" s="8" t="s">
+      <c r="F96" s="9" t="s">
         <v>87</v>
       </c>
       <c r="G96" s="7">
@@ -7021,23 +7039,23 @@
       <c r="B97" t="s">
         <v>53</v>
       </c>
-      <c r="C97" s="11">
-        <v>6000</v>
-      </c>
-      <c r="D97" s="11" t="s">
+      <c r="C97" s="7">
+        <v>15000</v>
+      </c>
+      <c r="D97" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E97" s="11">
-        <v>600000</v>
-      </c>
-      <c r="F97" s="11" t="s">
-        <v>63</v>
+      <c r="E97" s="8">
+        <v>2000000</v>
+      </c>
+      <c r="F97" s="8" t="s">
+        <v>87</v>
       </c>
       <c r="G97" s="7">
-        <v>1300000</v>
+        <v>4000000</v>
       </c>
       <c r="H97" s="7" t="s">
-        <v>87</v>
+        <v>77</v>
       </c>
       <c r="I97" s="4"/>
       <c r="J97" s="4"/>
@@ -7117,16 +7135,16 @@
       <c r="B99" t="s">
         <v>53</v>
       </c>
-      <c r="C99" s="7">
+      <c r="C99" s="11">
         <v>6000</v>
       </c>
-      <c r="D99" s="7" t="s">
+      <c r="D99" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E99" s="10">
+      <c r="E99" s="11">
         <v>600000</v>
       </c>
-      <c r="F99" s="10" t="s">
+      <c r="F99" s="11" t="s">
         <v>63</v>
       </c>
       <c r="G99" s="7">
@@ -7165,16 +7183,24 @@
       <c r="B100" t="s">
         <v>53</v>
       </c>
-      <c r="C100" s="19">
-        <v>2000</v>
-      </c>
-      <c r="D100" s="19" t="s">
+      <c r="C100" s="7">
+        <v>6000</v>
+      </c>
+      <c r="D100" s="7" t="s">
         <v>62</v>
       </c>
-      <c r="E100" s="4"/>
-      <c r="F100" s="4"/>
-      <c r="G100" s="4"/>
-      <c r="H100" s="4"/>
+      <c r="E100" s="10">
+        <v>600000</v>
+      </c>
+      <c r="F100" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="G100" s="7">
+        <v>1300000</v>
+      </c>
+      <c r="H100" s="7" t="s">
+        <v>87</v>
+      </c>
       <c r="I100" s="4"/>
       <c r="J100" s="4"/>
       <c r="K100" s="4"/>
@@ -7245,10 +7271,10 @@
       <c r="B102" t="s">
         <v>53</v>
       </c>
-      <c r="C102" s="15">
+      <c r="C102" s="19">
         <v>2000</v>
       </c>
-      <c r="D102" s="15" t="s">
+      <c r="D102" s="19" t="s">
         <v>62</v>
       </c>
       <c r="E102" s="4"/>
@@ -7325,10 +7351,10 @@
       <c r="B104" t="s">
         <v>53</v>
       </c>
-      <c r="C104" s="11">
+      <c r="C104" s="15">
         <v>2000</v>
       </c>
-      <c r="D104" s="11" t="s">
+      <c r="D104" s="15" t="s">
         <v>62</v>
       </c>
       <c r="E104" s="4"/>
@@ -7402,8 +7428,15 @@
       <c r="A106" t="s">
         <v>19</v>
       </c>
-      <c r="C106" s="4"/>
-      <c r="D106" s="4"/>
+      <c r="B106" t="s">
+        <v>53</v>
+      </c>
+      <c r="C106" s="11">
+        <v>2000</v>
+      </c>
+      <c r="D106" s="11" t="s">
+        <v>62</v>
+      </c>
       <c r="E106" s="4"/>
       <c r="F106" s="4"/>
       <c r="G106" s="4"/>
@@ -7435,57 +7468,22 @@
       <c r="A107" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B107" t="s">
-        <v>54</v>
-      </c>
-      <c r="C107" s="6">
-        <v>250</v>
-      </c>
-      <c r="D107" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E107" s="22">
-        <v>2500</v>
-      </c>
-      <c r="F107" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="G107" s="20">
-        <v>10000</v>
-      </c>
-      <c r="H107" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="I107" s="19">
-        <v>100000</v>
-      </c>
-      <c r="J107" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="K107" s="16">
-        <v>250000</v>
-      </c>
-      <c r="L107" s="16" t="s">
-        <v>87</v>
-      </c>
-      <c r="M107" s="15">
-        <v>750000</v>
-      </c>
-      <c r="N107" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="O107" s="9">
-        <v>2250000</v>
-      </c>
-      <c r="P107" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="Q107" s="7">
-        <v>6750000</v>
-      </c>
-      <c r="R107" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="C107" s="4"/>
+      <c r="D107" s="4"/>
+      <c r="E107" s="4"/>
+      <c r="F107" s="4"/>
+      <c r="G107" s="4"/>
+      <c r="H107" s="4"/>
+      <c r="I107" s="4"/>
+      <c r="J107" s="4"/>
+      <c r="K107" s="4"/>
+      <c r="L107" s="4"/>
+      <c r="M107" s="4"/>
+      <c r="N107" s="4"/>
+      <c r="O107" s="4"/>
+      <c r="P107" s="4"/>
+      <c r="Q107" s="4"/>
+      <c r="R107" s="4"/>
       <c r="S107" s="4"/>
       <c r="T107" s="4"/>
       <c r="U107" s="4"/>
@@ -7506,16 +7504,16 @@
       <c r="B108" t="s">
         <v>54</v>
       </c>
-      <c r="C108" s="20">
+      <c r="C108" s="6">
         <v>250</v>
       </c>
-      <c r="D108" s="20" t="s">
+      <c r="D108" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="E108" s="21">
+      <c r="E108" s="22">
         <v>2500</v>
       </c>
-      <c r="F108" s="21" t="s">
+      <c r="F108" s="22" t="s">
         <v>67</v>
       </c>
       <c r="G108" s="20">
@@ -7574,28 +7572,28 @@
       <c r="B109" t="s">
         <v>54</v>
       </c>
-      <c r="C109" s="16">
+      <c r="C109" s="20">
         <v>250</v>
       </c>
-      <c r="D109" s="16" t="s">
+      <c r="D109" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="E109" s="50">
+      <c r="E109" s="21">
         <v>2500</v>
       </c>
-      <c r="F109" s="50" t="s">
+      <c r="F109" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="G109" s="51">
+      <c r="G109" s="20">
         <v>10000</v>
       </c>
-      <c r="H109" s="51" t="s">
+      <c r="H109" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="I109" s="52">
+      <c r="I109" s="19">
         <v>100000</v>
       </c>
-      <c r="J109" s="52" t="s">
+      <c r="J109" s="19" t="s">
         <v>88</v>
       </c>
       <c r="K109" s="16">
@@ -7642,40 +7640,40 @@
       <c r="B110" t="s">
         <v>54</v>
       </c>
-      <c r="C110" s="13">
+      <c r="C110" s="16">
         <v>250</v>
       </c>
-      <c r="D110" s="13" t="s">
+      <c r="D110" s="16" t="s">
         <v>60</v>
       </c>
-      <c r="E110" s="30">
+      <c r="E110" s="50">
         <v>2500</v>
       </c>
-      <c r="F110" s="30" t="s">
+      <c r="F110" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="G110" s="31">
+      <c r="G110" s="51">
         <v>10000</v>
       </c>
-      <c r="H110" s="31" t="s">
+      <c r="H110" s="51" t="s">
         <v>61</v>
       </c>
-      <c r="I110" s="32">
+      <c r="I110" s="52">
         <v>100000</v>
       </c>
-      <c r="J110" s="32" t="s">
+      <c r="J110" s="52" t="s">
         <v>88</v>
       </c>
-      <c r="K110" s="44">
+      <c r="K110" s="16">
         <v>250000</v>
       </c>
-      <c r="L110" s="44" t="s">
+      <c r="L110" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="M110" s="17">
+      <c r="M110" s="15">
         <v>750000</v>
       </c>
-      <c r="N110" s="17" t="s">
+      <c r="N110" s="15" t="s">
         <v>77</v>
       </c>
       <c r="O110" s="9">
@@ -7710,66 +7708,58 @@
       <c r="B111" t="s">
         <v>54</v>
       </c>
-      <c r="C111" s="6">
-        <v>200</v>
-      </c>
-      <c r="D111" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E111" s="6">
-        <v>1000</v>
-      </c>
-      <c r="F111" s="6" t="s">
-        <v>85</v>
-      </c>
-      <c r="G111" s="6">
+      <c r="C111" s="13">
+        <v>250</v>
+      </c>
+      <c r="D111" s="13" t="s">
+        <v>60</v>
+      </c>
+      <c r="E111" s="30">
         <v>2500</v>
       </c>
-      <c r="H111" s="6" t="s">
-        <v>68</v>
-      </c>
-      <c r="I111" s="22">
-        <v>5000</v>
-      </c>
-      <c r="J111" s="22" t="s">
-        <v>66</v>
-      </c>
-      <c r="K111" s="20">
+      <c r="F111" s="30" t="s">
+        <v>67</v>
+      </c>
+      <c r="G111" s="31">
         <v>10000</v>
       </c>
-      <c r="L111" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="M111" s="19">
-        <v>80000</v>
-      </c>
-      <c r="N111" s="19" t="s">
-        <v>90</v>
-      </c>
-      <c r="O111" s="16">
-        <v>240000</v>
-      </c>
-      <c r="P111" s="16" t="s">
+      <c r="H111" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="I111" s="32">
+        <v>100000</v>
+      </c>
+      <c r="J111" s="32" t="s">
+        <v>88</v>
+      </c>
+      <c r="K111" s="44">
+        <v>250000</v>
+      </c>
+      <c r="L111" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="Q111" s="15">
-        <v>700000</v>
-      </c>
-      <c r="R111" s="15" t="s">
-        <v>70</v>
-      </c>
-      <c r="S111" s="13">
-        <v>1500000</v>
-      </c>
-      <c r="T111" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="U111" s="11">
-        <v>2000000</v>
-      </c>
-      <c r="V111" s="11" t="s">
-        <v>72</v>
-      </c>
+      <c r="M111" s="17">
+        <v>750000</v>
+      </c>
+      <c r="N111" s="17" t="s">
+        <v>77</v>
+      </c>
+      <c r="O111" s="9">
+        <v>2250000</v>
+      </c>
+      <c r="P111" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="Q111" s="7">
+        <v>6750000</v>
+      </c>
+      <c r="R111" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="S111" s="4"/>
+      <c r="T111" s="4"/>
+      <c r="U111" s="4"/>
+      <c r="V111" s="4"/>
       <c r="W111" s="4"/>
       <c r="X111" s="4"/>
       <c r="Y111" s="4"/>
@@ -7786,22 +7776,22 @@
       <c r="B112" t="s">
         <v>54</v>
       </c>
-      <c r="C112" s="22">
+      <c r="C112" s="6">
         <v>200</v>
       </c>
-      <c r="D112" s="22" t="s">
+      <c r="D112" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E112" s="57">
+      <c r="E112" s="6">
         <v>1000</v>
       </c>
-      <c r="F112" s="57" t="s">
+      <c r="F112" s="6" t="s">
         <v>85</v>
       </c>
-      <c r="G112" s="57">
+      <c r="G112" s="6">
         <v>2500</v>
       </c>
-      <c r="H112" s="57" t="s">
+      <c r="H112" s="6" t="s">
         <v>68</v>
       </c>
       <c r="I112" s="22">
@@ -7862,34 +7852,34 @@
       <c r="B113" t="s">
         <v>54</v>
       </c>
-      <c r="C113" s="19">
+      <c r="C113" s="22">
         <v>200</v>
       </c>
-      <c r="D113" s="19" t="s">
+      <c r="D113" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="E113" s="56">
+      <c r="E113" s="57">
         <v>1000</v>
       </c>
-      <c r="F113" s="56" t="s">
+      <c r="F113" s="57" t="s">
         <v>85</v>
       </c>
-      <c r="G113" s="56">
+      <c r="G113" s="57">
         <v>2500</v>
       </c>
-      <c r="H113" s="56" t="s">
+      <c r="H113" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="I113" s="23">
+      <c r="I113" s="22">
         <v>5000</v>
       </c>
-      <c r="J113" s="23" t="s">
+      <c r="J113" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="K113" s="24">
+      <c r="K113" s="20">
         <v>10000</v>
       </c>
-      <c r="L113" s="24" t="s">
+      <c r="L113" s="20" t="s">
         <v>89</v>
       </c>
       <c r="M113" s="19">
@@ -7938,52 +7928,52 @@
       <c r="B114" t="s">
         <v>54</v>
       </c>
-      <c r="C114" s="13">
+      <c r="C114" s="19">
         <v>200</v>
       </c>
-      <c r="D114" s="13" t="s">
+      <c r="D114" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E114" s="5">
+      <c r="E114" s="56">
         <v>1000</v>
       </c>
-      <c r="F114" s="5" t="s">
+      <c r="F114" s="56" t="s">
         <v>85</v>
       </c>
-      <c r="G114" s="5">
+      <c r="G114" s="56">
         <v>2500</v>
       </c>
-      <c r="H114" s="5" t="s">
+      <c r="H114" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="I114" s="30">
+      <c r="I114" s="23">
         <v>5000</v>
       </c>
-      <c r="J114" s="30" t="s">
+      <c r="J114" s="23" t="s">
         <v>66</v>
       </c>
-      <c r="K114" s="31">
+      <c r="K114" s="24">
         <v>10000</v>
       </c>
-      <c r="L114" s="31" t="s">
+      <c r="L114" s="24" t="s">
         <v>89</v>
       </c>
-      <c r="M114" s="32">
+      <c r="M114" s="19">
         <v>80000</v>
       </c>
-      <c r="N114" s="32" t="s">
+      <c r="N114" s="19" t="s">
         <v>90</v>
       </c>
-      <c r="O114" s="44">
+      <c r="O114" s="16">
         <v>240000</v>
       </c>
-      <c r="P114" s="44" t="s">
+      <c r="P114" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="Q114" s="17">
+      <c r="Q114" s="15">
         <v>700000</v>
       </c>
-      <c r="R114" s="17" t="s">
+      <c r="R114" s="15" t="s">
         <v>70</v>
       </c>
       <c r="S114" s="13">
@@ -8012,52 +8002,68 @@
         <v>21</v>
       </c>
       <c r="B115" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C115" s="13">
-        <v>750000</v>
+        <v>200</v>
       </c>
       <c r="D115" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="E115" s="13">
-        <v>1250000</v>
-      </c>
-      <c r="F115" s="13" t="s">
-        <v>58</v>
-      </c>
-      <c r="G115" s="11">
-        <v>1750000</v>
-      </c>
-      <c r="H115" s="11" t="s">
+        <v>59</v>
+      </c>
+      <c r="E115" s="5">
+        <v>1000</v>
+      </c>
+      <c r="F115" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="G115" s="5">
+        <v>2500</v>
+      </c>
+      <c r="H115" s="5" t="s">
+        <v>68</v>
+      </c>
+      <c r="I115" s="30">
+        <v>5000</v>
+      </c>
+      <c r="J115" s="30" t="s">
+        <v>66</v>
+      </c>
+      <c r="K115" s="31">
+        <v>10000</v>
+      </c>
+      <c r="L115" s="31" t="s">
+        <v>89</v>
+      </c>
+      <c r="M115" s="32">
+        <v>80000</v>
+      </c>
+      <c r="N115" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="O115" s="44">
+        <v>240000</v>
+      </c>
+      <c r="P115" s="44" t="s">
+        <v>87</v>
+      </c>
+      <c r="Q115" s="17">
+        <v>700000</v>
+      </c>
+      <c r="R115" s="17" t="s">
+        <v>70</v>
+      </c>
+      <c r="S115" s="13">
+        <v>1500000</v>
+      </c>
+      <c r="T115" s="13" t="s">
+        <v>71</v>
+      </c>
+      <c r="U115" s="11">
+        <v>2000000</v>
+      </c>
+      <c r="V115" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="I115" s="11">
-        <v>2250000</v>
-      </c>
-      <c r="J115" s="11" t="s">
-        <v>76</v>
-      </c>
-      <c r="K115" s="9">
-        <v>2750000</v>
-      </c>
-      <c r="L115" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="M115" s="9">
-        <v>3500000</v>
-      </c>
-      <c r="N115" s="9" t="s">
-        <v>78</v>
-      </c>
-      <c r="O115" s="4"/>
-      <c r="P115" s="4"/>
-      <c r="Q115" s="4"/>
-      <c r="R115" s="4"/>
-      <c r="S115" s="4"/>
-      <c r="T115" s="4"/>
-      <c r="U115" s="4"/>
-      <c r="V115" s="4"/>
       <c r="W115" s="4"/>
       <c r="X115" s="4"/>
       <c r="Y115" s="4"/>
@@ -8074,16 +8080,16 @@
       <c r="B116" t="s">
         <v>55</v>
       </c>
-      <c r="C116" s="11">
+      <c r="C116" s="13">
         <v>750000</v>
       </c>
-      <c r="D116" s="11" t="s">
+      <c r="D116" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="E116" s="37">
+      <c r="E116" s="13">
         <v>1250000</v>
       </c>
-      <c r="F116" s="37" t="s">
+      <c r="F116" s="13" t="s">
         <v>58</v>
       </c>
       <c r="G116" s="11">
@@ -8131,18 +8137,45 @@
       <c r="A117" t="s">
         <v>22</v>
       </c>
-      <c r="C117" s="4"/>
-      <c r="D117" s="4"/>
-      <c r="E117" s="4"/>
-      <c r="F117" s="4"/>
-      <c r="G117" s="4"/>
-      <c r="H117" s="4"/>
-      <c r="I117" s="4"/>
-      <c r="J117" s="4"/>
-      <c r="K117" s="4"/>
-      <c r="L117" s="4"/>
-      <c r="M117" s="4"/>
-      <c r="N117" s="4"/>
+      <c r="B117" t="s">
+        <v>55</v>
+      </c>
+      <c r="C117" s="11">
+        <v>750000</v>
+      </c>
+      <c r="D117" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="E117" s="37">
+        <v>1250000</v>
+      </c>
+      <c r="F117" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="G117" s="11">
+        <v>1750000</v>
+      </c>
+      <c r="H117" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="I117" s="11">
+        <v>2250000</v>
+      </c>
+      <c r="J117" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="K117" s="9">
+        <v>2750000</v>
+      </c>
+      <c r="L117" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="M117" s="9">
+        <v>3500000</v>
+      </c>
+      <c r="N117" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="O117" s="4"/>
       <c r="P117" s="4"/>
       <c r="Q117" s="4"/>
@@ -8164,81 +8197,30 @@
       <c r="A118" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B118" t="s">
-        <v>54</v>
-      </c>
-      <c r="C118" s="6">
-        <v>150</v>
-      </c>
-      <c r="D118" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E118" s="6">
-        <v>300</v>
-      </c>
-      <c r="F118" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G118" s="22">
-        <v>700</v>
-      </c>
-      <c r="H118" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="I118" s="22">
-        <v>1400</v>
-      </c>
-      <c r="J118" s="22" t="s">
-        <v>67</v>
-      </c>
-      <c r="K118" s="20">
-        <v>3000</v>
-      </c>
-      <c r="L118" s="20" t="s">
-        <v>68</v>
-      </c>
-      <c r="M118" s="20">
-        <v>7000</v>
-      </c>
-      <c r="N118" s="20" t="s">
-        <v>63</v>
-      </c>
-      <c r="O118" s="19">
-        <v>14000</v>
-      </c>
-      <c r="P118" s="19" t="s">
-        <v>69</v>
-      </c>
-      <c r="Q118" s="19">
-        <v>28000</v>
-      </c>
-      <c r="R118" s="19" t="s">
-        <v>87</v>
-      </c>
-      <c r="S118" s="16">
-        <v>56000</v>
-      </c>
-      <c r="T118" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="U118" s="16">
-        <v>84000</v>
-      </c>
-      <c r="V118" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="W118" s="13">
-        <v>168000</v>
-      </c>
-      <c r="X118" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y118" s="11">
-        <v>336000</v>
-      </c>
-      <c r="Z118" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="C118" s="4"/>
+      <c r="D118" s="4"/>
+      <c r="E118" s="4"/>
+      <c r="F118" s="4"/>
+      <c r="G118" s="4"/>
+      <c r="H118" s="4"/>
+      <c r="I118" s="4"/>
+      <c r="J118" s="4"/>
+      <c r="K118" s="4"/>
+      <c r="L118" s="4"/>
+      <c r="M118" s="4"/>
+      <c r="N118" s="4"/>
+      <c r="O118" s="4"/>
+      <c r="P118" s="4"/>
+      <c r="Q118" s="4"/>
+      <c r="R118" s="4"/>
+      <c r="S118" s="4"/>
+      <c r="T118" s="4"/>
+      <c r="U118" s="4"/>
+      <c r="V118" s="4"/>
+      <c r="W118" s="4"/>
+      <c r="X118" s="4"/>
+      <c r="Y118" s="4"/>
+      <c r="Z118" s="4"/>
       <c r="AA118" s="4"/>
       <c r="AB118" s="4"/>
       <c r="AC118" s="3"/>
@@ -8251,16 +8233,16 @@
       <c r="B119" t="s">
         <v>54</v>
       </c>
-      <c r="C119" s="22">
+      <c r="C119" s="6">
         <v>150</v>
       </c>
-      <c r="D119" s="22" t="s">
+      <c r="D119" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E119" s="57">
+      <c r="E119" s="6">
         <v>300</v>
       </c>
-      <c r="F119" s="57" t="s">
+      <c r="F119" s="6" t="s">
         <v>60</v>
       </c>
       <c r="G119" s="22">
@@ -8335,28 +8317,28 @@
       <c r="B120" t="s">
         <v>54</v>
       </c>
-      <c r="C120" s="20">
+      <c r="C120" s="22">
         <v>150</v>
       </c>
-      <c r="D120" s="20" t="s">
+      <c r="D120" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="E120" s="58">
+      <c r="E120" s="57">
         <v>300</v>
       </c>
-      <c r="F120" s="58" t="s">
+      <c r="F120" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="G120" s="21">
+      <c r="G120" s="22">
         <v>700</v>
       </c>
-      <c r="H120" s="21" t="s">
+      <c r="H120" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="I120" s="21">
+      <c r="I120" s="22">
         <v>1400</v>
       </c>
-      <c r="J120" s="21" t="s">
+      <c r="J120" s="22" t="s">
         <v>67</v>
       </c>
       <c r="K120" s="20">
@@ -8419,40 +8401,40 @@
       <c r="B121" t="s">
         <v>54</v>
       </c>
-      <c r="C121" s="19">
+      <c r="C121" s="20">
         <v>150</v>
       </c>
-      <c r="D121" s="19" t="s">
+      <c r="D121" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E121" s="56">
+      <c r="E121" s="58">
         <v>300</v>
       </c>
-      <c r="F121" s="56" t="s">
+      <c r="F121" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="G121" s="23">
+      <c r="G121" s="21">
         <v>700</v>
       </c>
-      <c r="H121" s="23" t="s">
+      <c r="H121" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="I121" s="23">
+      <c r="I121" s="21">
         <v>1400</v>
       </c>
-      <c r="J121" s="23" t="s">
+      <c r="J121" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="K121" s="24">
+      <c r="K121" s="20">
         <v>3000</v>
       </c>
-      <c r="L121" s="24" t="s">
+      <c r="L121" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="M121" s="24">
+      <c r="M121" s="20">
         <v>7000</v>
       </c>
-      <c r="N121" s="24" t="s">
+      <c r="N121" s="20" t="s">
         <v>63</v>
       </c>
       <c r="O121" s="19">
@@ -8503,52 +8485,52 @@
       <c r="B122" t="s">
         <v>54</v>
       </c>
-      <c r="C122" s="16">
+      <c r="C122" s="19">
         <v>150</v>
       </c>
-      <c r="D122" s="16" t="s">
+      <c r="D122" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E122" s="49">
+      <c r="E122" s="56">
         <v>300</v>
       </c>
-      <c r="F122" s="49" t="s">
+      <c r="F122" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="G122" s="50">
+      <c r="G122" s="23">
         <v>700</v>
       </c>
-      <c r="H122" s="50" t="s">
+      <c r="H122" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="I122" s="50">
+      <c r="I122" s="23">
         <v>1400</v>
       </c>
-      <c r="J122" s="50" t="s">
+      <c r="J122" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="K122" s="51">
+      <c r="K122" s="24">
         <v>3000</v>
       </c>
-      <c r="L122" s="51" t="s">
+      <c r="L122" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="M122" s="51">
+      <c r="M122" s="24">
         <v>7000</v>
       </c>
-      <c r="N122" s="51" t="s">
+      <c r="N122" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="O122" s="52">
+      <c r="O122" s="19">
         <v>14000</v>
       </c>
-      <c r="P122" s="52" t="s">
+      <c r="P122" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="Q122" s="52">
+      <c r="Q122" s="19">
         <v>28000</v>
       </c>
-      <c r="R122" s="52" t="s">
+      <c r="R122" s="19" t="s">
         <v>87</v>
       </c>
       <c r="S122" s="16">
@@ -8587,64 +8569,64 @@
       <c r="B123" t="s">
         <v>54</v>
       </c>
-      <c r="C123" s="15">
+      <c r="C123" s="16">
         <v>150</v>
       </c>
-      <c r="D123" s="15" t="s">
+      <c r="D123" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E123" s="75">
+      <c r="E123" s="49">
         <v>300</v>
       </c>
-      <c r="F123" s="75" t="s">
+      <c r="F123" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="G123" s="76">
+      <c r="G123" s="50">
         <v>700</v>
       </c>
-      <c r="H123" s="76" t="s">
+      <c r="H123" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="I123" s="76">
+      <c r="I123" s="50">
         <v>1400</v>
       </c>
-      <c r="J123" s="76" t="s">
+      <c r="J123" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="K123" s="77">
+      <c r="K123" s="51">
         <v>3000</v>
       </c>
-      <c r="L123" s="77" t="s">
+      <c r="L123" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="M123" s="77">
+      <c r="M123" s="51">
         <v>7000</v>
       </c>
-      <c r="N123" s="77" t="s">
+      <c r="N123" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="O123" s="78">
+      <c r="O123" s="52">
         <v>14000</v>
       </c>
-      <c r="P123" s="78" t="s">
+      <c r="P123" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="Q123" s="78">
+      <c r="Q123" s="52">
         <v>28000</v>
       </c>
-      <c r="R123" s="78" t="s">
+      <c r="R123" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="S123" s="55">
+      <c r="S123" s="16">
         <v>56000</v>
       </c>
-      <c r="T123" s="55" t="s">
+      <c r="T123" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="U123" s="55">
+      <c r="U123" s="16">
         <v>84000</v>
       </c>
-      <c r="V123" s="55" t="s">
+      <c r="V123" s="16" t="s">
         <v>77</v>
       </c>
       <c r="W123" s="13">
@@ -8671,76 +8653,76 @@
       <c r="B124" t="s">
         <v>54</v>
       </c>
-      <c r="C124" s="7">
+      <c r="C124" s="15">
         <v>150</v>
       </c>
-      <c r="D124" s="7" t="s">
+      <c r="D124" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E124" s="59">
+      <c r="E124" s="75">
         <v>300</v>
       </c>
-      <c r="F124" s="59" t="s">
+      <c r="F124" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="G124" s="60">
+      <c r="G124" s="76">
         <v>700</v>
       </c>
-      <c r="H124" s="60" t="s">
+      <c r="H124" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="I124" s="60">
+      <c r="I124" s="76">
         <v>1400</v>
       </c>
-      <c r="J124" s="60" t="s">
+      <c r="J124" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="K124" s="61">
+      <c r="K124" s="77">
         <v>3000</v>
       </c>
-      <c r="L124" s="61" t="s">
+      <c r="L124" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="M124" s="61">
+      <c r="M124" s="77">
         <v>7000</v>
       </c>
-      <c r="N124" s="61" t="s">
+      <c r="N124" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="O124" s="62">
+      <c r="O124" s="78">
         <v>14000</v>
       </c>
-      <c r="P124" s="62" t="s">
+      <c r="P124" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="Q124" s="62">
+      <c r="Q124" s="78">
         <v>28000</v>
       </c>
-      <c r="R124" s="62" t="s">
+      <c r="R124" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="S124" s="47">
+      <c r="S124" s="55">
         <v>56000</v>
       </c>
-      <c r="T124" s="47" t="s">
+      <c r="T124" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="U124" s="47">
+      <c r="U124" s="55">
         <v>84000</v>
       </c>
-      <c r="V124" s="47" t="s">
+      <c r="V124" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="W124" s="63">
+      <c r="W124" s="13">
         <v>168000</v>
       </c>
-      <c r="X124" s="63" t="s">
+      <c r="X124" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="Y124" s="64">
+      <c r="Y124" s="11">
         <v>336000</v>
       </c>
-      <c r="Z124" s="64" t="s">
+      <c r="Z124" s="11" t="s">
         <v>58</v>
       </c>
       <c r="AA124" s="4"/>
@@ -8755,74 +8737,78 @@
       <c r="B125" t="s">
         <v>54</v>
       </c>
-      <c r="C125" s="6">
+      <c r="C125" s="7">
+        <v>150</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E125" s="59">
         <v>300</v>
       </c>
-      <c r="D125" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E125" s="22">
-        <v>750</v>
-      </c>
-      <c r="F125" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G125" s="22">
-        <v>1500</v>
-      </c>
-      <c r="H125" s="22" t="s">
+      <c r="F125" s="59" t="s">
+        <v>60</v>
+      </c>
+      <c r="G125" s="60">
+        <v>700</v>
+      </c>
+      <c r="H125" s="60" t="s">
+        <v>85</v>
+      </c>
+      <c r="I125" s="60">
+        <v>1400</v>
+      </c>
+      <c r="J125" s="60" t="s">
         <v>67</v>
       </c>
-      <c r="I125" s="20">
+      <c r="K125" s="61">
         <v>3000</v>
       </c>
-      <c r="J125" s="20" t="s">
+      <c r="L125" s="61" t="s">
         <v>68</v>
       </c>
-      <c r="K125" s="20">
-        <v>6000</v>
-      </c>
-      <c r="L125" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="M125" s="20">
-        <v>12000</v>
-      </c>
-      <c r="N125" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="O125" s="19">
-        <v>25000</v>
-      </c>
-      <c r="P125" s="19" t="s">
+      <c r="M125" s="61">
+        <v>7000</v>
+      </c>
+      <c r="N125" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="Q125" s="19">
-        <v>50000</v>
-      </c>
-      <c r="R125" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="S125" s="16">
-        <v>100000</v>
-      </c>
-      <c r="T125" s="16" t="s">
+      <c r="O125" s="62">
+        <v>14000</v>
+      </c>
+      <c r="P125" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="U125" s="15">
-        <v>250000</v>
-      </c>
-      <c r="V125" s="15" t="s">
+      <c r="Q125" s="62">
+        <v>28000</v>
+      </c>
+      <c r="R125" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="W125" s="13">
-        <v>500000</v>
-      </c>
-      <c r="X125" s="13" t="s">
+      <c r="S125" s="47">
+        <v>56000</v>
+      </c>
+      <c r="T125" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="Y125" s="4"/>
-      <c r="Z125" s="4"/>
+      <c r="U125" s="47">
+        <v>84000</v>
+      </c>
+      <c r="V125" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="W125" s="63">
+        <v>168000</v>
+      </c>
+      <c r="X125" s="63" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y125" s="64">
+        <v>336000</v>
+      </c>
+      <c r="Z125" s="64" t="s">
+        <v>58</v>
+      </c>
       <c r="AA125" s="4"/>
       <c r="AB125" s="4"/>
       <c r="AC125" s="3"/>
@@ -8835,22 +8821,22 @@
       <c r="B126" t="s">
         <v>54</v>
       </c>
-      <c r="C126" s="20">
+      <c r="C126" s="6">
         <v>300</v>
       </c>
-      <c r="D126" s="20" t="s">
+      <c r="D126" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E126" s="21">
+      <c r="E126" s="22">
         <v>750</v>
       </c>
-      <c r="F126" s="21" t="s">
+      <c r="F126" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G126" s="21">
+      <c r="G126" s="22">
         <v>1500</v>
       </c>
-      <c r="H126" s="21" t="s">
+      <c r="H126" s="22" t="s">
         <v>67</v>
       </c>
       <c r="I126" s="20">
@@ -8915,70 +8901,70 @@
       <c r="B127" t="s">
         <v>54</v>
       </c>
-      <c r="C127" s="11">
+      <c r="C127" s="20">
         <v>300</v>
       </c>
-      <c r="D127" s="11" t="s">
+      <c r="D127" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E127" s="65">
+      <c r="E127" s="21">
         <v>750</v>
       </c>
-      <c r="F127" s="65" t="s">
+      <c r="F127" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G127" s="65">
+      <c r="G127" s="21">
         <v>1500</v>
       </c>
-      <c r="H127" s="65" t="s">
+      <c r="H127" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I127" s="66">
+      <c r="I127" s="20">
         <v>3000</v>
       </c>
-      <c r="J127" s="66" t="s">
+      <c r="J127" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="K127" s="66">
+      <c r="K127" s="20">
         <v>6000</v>
       </c>
-      <c r="L127" s="66" t="s">
+      <c r="L127" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="M127" s="66">
+      <c r="M127" s="20">
         <v>12000</v>
       </c>
-      <c r="N127" s="66" t="s">
+      <c r="N127" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="O127" s="67">
+      <c r="O127" s="19">
         <v>25000</v>
       </c>
-      <c r="P127" s="67" t="s">
+      <c r="P127" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Q127" s="67">
+      <c r="Q127" s="19">
         <v>50000</v>
       </c>
-      <c r="R127" s="67" t="s">
+      <c r="R127" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="S127" s="45">
+      <c r="S127" s="16">
         <v>100000</v>
       </c>
-      <c r="T127" s="45" t="s">
+      <c r="T127" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="U127" s="68">
+      <c r="U127" s="15">
         <v>250000</v>
       </c>
-      <c r="V127" s="68" t="s">
+      <c r="V127" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="W127" s="69">
+      <c r="W127" s="13">
         <v>500000</v>
       </c>
-      <c r="X127" s="69" t="s">
+      <c r="X127" s="13" t="s">
         <v>70</v>
       </c>
       <c r="Y127" s="4"/>
@@ -8995,70 +8981,70 @@
       <c r="B128" t="s">
         <v>54</v>
       </c>
-      <c r="C128" s="9">
+      <c r="C128" s="11">
         <v>300</v>
       </c>
-      <c r="D128" s="9" t="s">
+      <c r="D128" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E128" s="70">
+      <c r="E128" s="65">
         <v>750</v>
       </c>
-      <c r="F128" s="70" t="s">
+      <c r="F128" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="G128" s="70">
+      <c r="G128" s="65">
         <v>1500</v>
       </c>
-      <c r="H128" s="70" t="s">
+      <c r="H128" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="I128" s="71">
+      <c r="I128" s="66">
         <v>3000</v>
       </c>
-      <c r="J128" s="71" t="s">
+      <c r="J128" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="K128" s="71">
+      <c r="K128" s="66">
         <v>6000</v>
       </c>
-      <c r="L128" s="71" t="s">
+      <c r="L128" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="M128" s="71">
+      <c r="M128" s="66">
         <v>12000</v>
       </c>
-      <c r="N128" s="71" t="s">
+      <c r="N128" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="O128" s="72">
+      <c r="O128" s="67">
         <v>25000</v>
       </c>
-      <c r="P128" s="72" t="s">
+      <c r="P128" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="Q128" s="72">
+      <c r="Q128" s="67">
         <v>50000</v>
       </c>
-      <c r="R128" s="72" t="s">
+      <c r="R128" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="S128" s="46">
+      <c r="S128" s="45">
         <v>100000</v>
       </c>
-      <c r="T128" s="46" t="s">
+      <c r="T128" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="U128" s="73">
+      <c r="U128" s="68">
         <v>250000</v>
       </c>
-      <c r="V128" s="73" t="s">
+      <c r="V128" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="W128" s="74">
+      <c r="W128" s="69">
         <v>500000</v>
       </c>
-      <c r="X128" s="74" t="s">
+      <c r="X128" s="69" t="s">
         <v>70</v>
       </c>
       <c r="Y128" s="4"/>
@@ -9073,80 +9059,76 @@
         <v>46</v>
       </c>
       <c r="B129" t="s">
-        <v>53</v>
-      </c>
-      <c r="C129" s="6">
-        <v>150</v>
-      </c>
-      <c r="D129" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C129" s="9">
+        <v>300</v>
+      </c>
+      <c r="D129" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="E129" s="6">
-        <v>300</v>
-      </c>
-      <c r="F129" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="G129" s="22">
-        <v>700</v>
-      </c>
-      <c r="H129" s="22" t="s">
-        <v>85</v>
-      </c>
-      <c r="I129" s="22">
-        <v>1400</v>
-      </c>
-      <c r="J129" s="22" t="s">
+      <c r="E129" s="70">
+        <v>750</v>
+      </c>
+      <c r="F129" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="G129" s="70">
+        <v>1500</v>
+      </c>
+      <c r="H129" s="70" t="s">
         <v>67</v>
       </c>
-      <c r="K129" s="20">
-        <v>3500</v>
-      </c>
-      <c r="L129" s="20" t="s">
+      <c r="I129" s="71">
+        <v>3000</v>
+      </c>
+      <c r="J129" s="71" t="s">
         <v>68</v>
       </c>
-      <c r="M129" s="20">
-        <v>7000</v>
-      </c>
-      <c r="N129" s="20" t="s">
+      <c r="K129" s="71">
+        <v>6000</v>
+      </c>
+      <c r="L129" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="M129" s="71">
+        <v>12000</v>
+      </c>
+      <c r="N129" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="O129" s="72">
+        <v>25000</v>
+      </c>
+      <c r="P129" s="72" t="s">
         <v>63</v>
       </c>
-      <c r="O129" s="19">
-        <v>14000</v>
-      </c>
-      <c r="P129" s="19" t="s">
+      <c r="Q129" s="72">
+        <v>50000</v>
+      </c>
+      <c r="R129" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="S129" s="46">
+        <v>100000</v>
+      </c>
+      <c r="T129" s="46" t="s">
         <v>69</v>
       </c>
-      <c r="Q129" s="19">
-        <v>28000</v>
-      </c>
-      <c r="R129" s="19" t="s">
+      <c r="U129" s="73">
+        <v>250000</v>
+      </c>
+      <c r="V129" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="S129" s="16">
-        <v>56000</v>
-      </c>
-      <c r="T129" s="16" t="s">
+      <c r="W129" s="74">
+        <v>500000</v>
+      </c>
+      <c r="X129" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="U129" s="16">
-        <v>84000</v>
-      </c>
-      <c r="V129" s="16" t="s">
-        <v>77</v>
-      </c>
-      <c r="W129" s="13">
-        <v>168000</v>
-      </c>
-      <c r="X129" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="Y129" s="11">
-        <v>336000</v>
-      </c>
-      <c r="Z129" s="11" t="s">
-        <v>58</v>
-      </c>
+      <c r="Y129" s="4"/>
+      <c r="Z129" s="4"/>
       <c r="AA129" s="4"/>
       <c r="AB129" s="4"/>
       <c r="AC129" s="3"/>
@@ -9159,16 +9141,16 @@
       <c r="B130" t="s">
         <v>53</v>
       </c>
-      <c r="C130" s="22">
+      <c r="C130" s="6">
         <v>150</v>
       </c>
-      <c r="D130" s="22" t="s">
+      <c r="D130" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E130" s="57">
+      <c r="E130" s="6">
         <v>300</v>
       </c>
-      <c r="F130" s="57" t="s">
+      <c r="F130" s="6" t="s">
         <v>60</v>
       </c>
       <c r="G130" s="22">
@@ -9243,28 +9225,28 @@
       <c r="B131" t="s">
         <v>53</v>
       </c>
-      <c r="C131" s="20">
+      <c r="C131" s="22">
         <v>150</v>
       </c>
-      <c r="D131" s="20" t="s">
+      <c r="D131" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="E131" s="58">
+      <c r="E131" s="57">
         <v>300</v>
       </c>
-      <c r="F131" s="58" t="s">
+      <c r="F131" s="57" t="s">
         <v>60</v>
       </c>
-      <c r="G131" s="21">
+      <c r="G131" s="22">
         <v>700</v>
       </c>
-      <c r="H131" s="21" t="s">
+      <c r="H131" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="I131" s="21">
+      <c r="I131" s="22">
         <v>1400</v>
       </c>
-      <c r="J131" s="21" t="s">
+      <c r="J131" s="22" t="s">
         <v>67</v>
       </c>
       <c r="K131" s="20">
@@ -9327,40 +9309,40 @@
       <c r="B132" t="s">
         <v>53</v>
       </c>
-      <c r="C132" s="19">
+      <c r="C132" s="20">
         <v>150</v>
       </c>
-      <c r="D132" s="19" t="s">
+      <c r="D132" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E132" s="56">
+      <c r="E132" s="58">
         <v>300</v>
       </c>
-      <c r="F132" s="56" t="s">
+      <c r="F132" s="58" t="s">
         <v>60</v>
       </c>
-      <c r="G132" s="23">
+      <c r="G132" s="21">
         <v>700</v>
       </c>
-      <c r="H132" s="23" t="s">
+      <c r="H132" s="21" t="s">
         <v>85</v>
       </c>
-      <c r="I132" s="23">
+      <c r="I132" s="21">
         <v>1400</v>
       </c>
-      <c r="J132" s="23" t="s">
+      <c r="J132" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="K132" s="24">
+      <c r="K132" s="20">
         <v>3500</v>
       </c>
-      <c r="L132" s="24" t="s">
+      <c r="L132" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="M132" s="24">
+      <c r="M132" s="20">
         <v>7000</v>
       </c>
-      <c r="N132" s="24" t="s">
+      <c r="N132" s="20" t="s">
         <v>63</v>
       </c>
       <c r="O132" s="19">
@@ -9411,52 +9393,52 @@
       <c r="B133" t="s">
         <v>53</v>
       </c>
-      <c r="C133" s="16">
+      <c r="C133" s="19">
         <v>150</v>
       </c>
-      <c r="D133" s="16" t="s">
+      <c r="D133" s="19" t="s">
         <v>59</v>
       </c>
-      <c r="E133" s="49">
+      <c r="E133" s="56">
         <v>300</v>
       </c>
-      <c r="F133" s="49" t="s">
+      <c r="F133" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="G133" s="50">
+      <c r="G133" s="23">
         <v>700</v>
       </c>
-      <c r="H133" s="50" t="s">
+      <c r="H133" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="I133" s="50">
+      <c r="I133" s="23">
         <v>1400</v>
       </c>
-      <c r="J133" s="50" t="s">
+      <c r="J133" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="K133" s="51">
+      <c r="K133" s="24">
         <v>3500</v>
       </c>
-      <c r="L133" s="51" t="s">
+      <c r="L133" s="24" t="s">
         <v>68</v>
       </c>
-      <c r="M133" s="51">
+      <c r="M133" s="24">
         <v>7000</v>
       </c>
-      <c r="N133" s="51" t="s">
+      <c r="N133" s="24" t="s">
         <v>63</v>
       </c>
-      <c r="O133" s="52">
+      <c r="O133" s="19">
         <v>14000</v>
       </c>
-      <c r="P133" s="52" t="s">
+      <c r="P133" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="Q133" s="52">
+      <c r="Q133" s="19">
         <v>28000</v>
       </c>
-      <c r="R133" s="52" t="s">
+      <c r="R133" s="19" t="s">
         <v>87</v>
       </c>
       <c r="S133" s="16">
@@ -9495,64 +9477,64 @@
       <c r="B134" t="s">
         <v>53</v>
       </c>
-      <c r="C134" s="15">
+      <c r="C134" s="16">
         <v>150</v>
       </c>
-      <c r="D134" s="15" t="s">
+      <c r="D134" s="16" t="s">
         <v>59</v>
       </c>
-      <c r="E134" s="75">
+      <c r="E134" s="49">
         <v>300</v>
       </c>
-      <c r="F134" s="75" t="s">
+      <c r="F134" s="49" t="s">
         <v>60</v>
       </c>
-      <c r="G134" s="76">
+      <c r="G134" s="50">
         <v>700</v>
       </c>
-      <c r="H134" s="76" t="s">
+      <c r="H134" s="50" t="s">
         <v>85</v>
       </c>
-      <c r="I134" s="76">
+      <c r="I134" s="50">
         <v>1400</v>
       </c>
-      <c r="J134" s="76" t="s">
+      <c r="J134" s="50" t="s">
         <v>67</v>
       </c>
-      <c r="K134" s="77">
+      <c r="K134" s="51">
         <v>3500</v>
       </c>
-      <c r="L134" s="77" t="s">
+      <c r="L134" s="51" t="s">
         <v>68</v>
       </c>
-      <c r="M134" s="77">
+      <c r="M134" s="51">
         <v>7000</v>
       </c>
-      <c r="N134" s="77" t="s">
+      <c r="N134" s="51" t="s">
         <v>63</v>
       </c>
-      <c r="O134" s="78">
+      <c r="O134" s="52">
         <v>14000</v>
       </c>
-      <c r="P134" s="78" t="s">
+      <c r="P134" s="52" t="s">
         <v>69</v>
       </c>
-      <c r="Q134" s="78">
+      <c r="Q134" s="52">
         <v>28000</v>
       </c>
-      <c r="R134" s="78" t="s">
+      <c r="R134" s="52" t="s">
         <v>87</v>
       </c>
-      <c r="S134" s="55">
+      <c r="S134" s="16">
         <v>56000</v>
       </c>
-      <c r="T134" s="55" t="s">
+      <c r="T134" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="U134" s="55">
+      <c r="U134" s="16">
         <v>84000</v>
       </c>
-      <c r="V134" s="55" t="s">
+      <c r="V134" s="16" t="s">
         <v>77</v>
       </c>
       <c r="W134" s="13">
@@ -9579,76 +9561,76 @@
       <c r="B135" t="s">
         <v>53</v>
       </c>
-      <c r="C135" s="7">
+      <c r="C135" s="15">
         <v>150</v>
       </c>
-      <c r="D135" s="7" t="s">
+      <c r="D135" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="E135" s="53">
+      <c r="E135" s="75">
         <v>300</v>
       </c>
-      <c r="F135" s="53" t="s">
+      <c r="F135" s="75" t="s">
         <v>60</v>
       </c>
-      <c r="G135" s="28">
+      <c r="G135" s="76">
         <v>700</v>
       </c>
-      <c r="H135" s="28" t="s">
+      <c r="H135" s="76" t="s">
         <v>85</v>
       </c>
-      <c r="I135" s="28">
+      <c r="I135" s="76">
         <v>1400</v>
       </c>
-      <c r="J135" s="28" t="s">
+      <c r="J135" s="76" t="s">
         <v>67</v>
       </c>
-      <c r="K135" s="29">
+      <c r="K135" s="77">
         <v>3500</v>
       </c>
-      <c r="L135" s="29" t="s">
+      <c r="L135" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="M135" s="29">
+      <c r="M135" s="77">
         <v>7000</v>
       </c>
-      <c r="N135" s="29" t="s">
+      <c r="N135" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="O135" s="18">
+      <c r="O135" s="78">
         <v>14000</v>
       </c>
-      <c r="P135" s="18" t="s">
+      <c r="P135" s="78" t="s">
         <v>69</v>
       </c>
-      <c r="Q135" s="18">
+      <c r="Q135" s="78">
         <v>28000</v>
       </c>
-      <c r="R135" s="18" t="s">
+      <c r="R135" s="78" t="s">
         <v>87</v>
       </c>
-      <c r="S135" s="47">
+      <c r="S135" s="55">
         <v>56000</v>
       </c>
-      <c r="T135" s="47" t="s">
+      <c r="T135" s="55" t="s">
         <v>70</v>
       </c>
-      <c r="U135" s="47">
+      <c r="U135" s="55">
         <v>84000</v>
       </c>
-      <c r="V135" s="47" t="s">
+      <c r="V135" s="55" t="s">
         <v>77</v>
       </c>
-      <c r="W135" s="12">
+      <c r="W135" s="13">
         <v>168000</v>
       </c>
-      <c r="X135" s="12" t="s">
+      <c r="X135" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="Y135" s="10">
+      <c r="Y135" s="11">
         <v>336000</v>
       </c>
-      <c r="Z135" s="10" t="s">
+      <c r="Z135" s="11" t="s">
         <v>58</v>
       </c>
       <c r="AA135" s="4"/>
@@ -9663,74 +9645,78 @@
       <c r="B136" t="s">
         <v>53</v>
       </c>
-      <c r="C136" s="6">
+      <c r="C136" s="7">
+        <v>150</v>
+      </c>
+      <c r="D136" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E136" s="53">
         <v>300</v>
       </c>
-      <c r="D136" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="E136" s="22">
-        <v>750</v>
-      </c>
-      <c r="F136" s="22" t="s">
-        <v>64</v>
-      </c>
-      <c r="G136" s="22">
-        <v>1500</v>
-      </c>
-      <c r="H136" s="22" t="s">
+      <c r="F136" s="53" t="s">
+        <v>60</v>
+      </c>
+      <c r="G136" s="28">
+        <v>700</v>
+      </c>
+      <c r="H136" s="28" t="s">
+        <v>85</v>
+      </c>
+      <c r="I136" s="28">
+        <v>1400</v>
+      </c>
+      <c r="J136" s="28" t="s">
         <v>67</v>
       </c>
-      <c r="I136" s="20">
-        <v>3000</v>
-      </c>
-      <c r="J136" s="20" t="s">
+      <c r="K136" s="29">
+        <v>3500</v>
+      </c>
+      <c r="L136" s="29" t="s">
         <v>68</v>
       </c>
-      <c r="K136" s="20">
-        <v>6000</v>
-      </c>
-      <c r="L136" s="20" t="s">
-        <v>61</v>
-      </c>
-      <c r="M136" s="20">
-        <v>12000</v>
-      </c>
-      <c r="N136" s="20" t="s">
-        <v>66</v>
-      </c>
-      <c r="O136" s="19">
-        <v>25000</v>
-      </c>
-      <c r="P136" s="19" t="s">
+      <c r="M136" s="29">
+        <v>7000</v>
+      </c>
+      <c r="N136" s="29" t="s">
         <v>63</v>
       </c>
-      <c r="Q136" s="19">
-        <v>50000</v>
-      </c>
-      <c r="R136" s="19" t="s">
-        <v>88</v>
-      </c>
-      <c r="S136" s="16">
-        <v>100000</v>
-      </c>
-      <c r="T136" s="16" t="s">
+      <c r="O136" s="18">
+        <v>14000</v>
+      </c>
+      <c r="P136" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="U136" s="15">
-        <v>250000</v>
-      </c>
-      <c r="V136" s="15" t="s">
+      <c r="Q136" s="18">
+        <v>28000</v>
+      </c>
+      <c r="R136" s="18" t="s">
         <v>87</v>
       </c>
-      <c r="W136" s="13">
-        <v>500000</v>
-      </c>
-      <c r="X136" s="13" t="s">
+      <c r="S136" s="47">
+        <v>56000</v>
+      </c>
+      <c r="T136" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="Y136" s="4"/>
-      <c r="Z136" s="4"/>
+      <c r="U136" s="47">
+        <v>84000</v>
+      </c>
+      <c r="V136" s="47" t="s">
+        <v>77</v>
+      </c>
+      <c r="W136" s="12">
+        <v>168000</v>
+      </c>
+      <c r="X136" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y136" s="10">
+        <v>336000</v>
+      </c>
+      <c r="Z136" s="10" t="s">
+        <v>58</v>
+      </c>
       <c r="AA136" s="4"/>
       <c r="AB136" s="4"/>
       <c r="AC136" s="3"/>
@@ -9743,22 +9729,22 @@
       <c r="B137" t="s">
         <v>53</v>
       </c>
-      <c r="C137" s="20">
+      <c r="C137" s="6">
         <v>300</v>
       </c>
-      <c r="D137" s="20" t="s">
+      <c r="D137" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="E137" s="21">
+      <c r="E137" s="22">
         <v>750</v>
       </c>
-      <c r="F137" s="21" t="s">
+      <c r="F137" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="G137" s="21">
+      <c r="G137" s="22">
         <v>1500</v>
       </c>
-      <c r="H137" s="21" t="s">
+      <c r="H137" s="22" t="s">
         <v>67</v>
       </c>
       <c r="I137" s="20">
@@ -9823,70 +9809,70 @@
       <c r="B138" t="s">
         <v>53</v>
       </c>
-      <c r="C138" s="11">
+      <c r="C138" s="20">
         <v>300</v>
       </c>
-      <c r="D138" s="11" t="s">
+      <c r="D138" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="E138" s="65">
+      <c r="E138" s="21">
         <v>750</v>
       </c>
-      <c r="F138" s="65" t="s">
+      <c r="F138" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="G138" s="65">
+      <c r="G138" s="21">
         <v>1500</v>
       </c>
-      <c r="H138" s="65" t="s">
+      <c r="H138" s="21" t="s">
         <v>67</v>
       </c>
-      <c r="I138" s="66">
+      <c r="I138" s="20">
         <v>3000</v>
       </c>
-      <c r="J138" s="66" t="s">
+      <c r="J138" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="K138" s="66">
+      <c r="K138" s="20">
         <v>6000</v>
       </c>
-      <c r="L138" s="66" t="s">
+      <c r="L138" s="20" t="s">
         <v>61</v>
       </c>
-      <c r="M138" s="66">
+      <c r="M138" s="20">
         <v>12000</v>
       </c>
-      <c r="N138" s="66" t="s">
+      <c r="N138" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="O138" s="67">
+      <c r="O138" s="19">
         <v>25000</v>
       </c>
-      <c r="P138" s="67" t="s">
+      <c r="P138" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="Q138" s="67">
+      <c r="Q138" s="19">
         <v>50000</v>
       </c>
-      <c r="R138" s="67" t="s">
+      <c r="R138" s="19" t="s">
         <v>88</v>
       </c>
-      <c r="S138" s="45">
+      <c r="S138" s="16">
         <v>100000</v>
       </c>
-      <c r="T138" s="45" t="s">
+      <c r="T138" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="U138" s="68">
+      <c r="U138" s="15">
         <v>250000</v>
       </c>
-      <c r="V138" s="68" t="s">
+      <c r="V138" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="W138" s="69">
+      <c r="W138" s="13">
         <v>500000</v>
       </c>
-      <c r="X138" s="69" t="s">
+      <c r="X138" s="13" t="s">
         <v>70</v>
       </c>
       <c r="Y138" s="4"/>
@@ -9903,70 +9889,70 @@
       <c r="B139" t="s">
         <v>53</v>
       </c>
-      <c r="C139" s="9">
+      <c r="C139" s="11">
         <v>300</v>
       </c>
-      <c r="D139" s="9" t="s">
+      <c r="D139" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="E139" s="70">
+      <c r="E139" s="65">
         <v>750</v>
       </c>
-      <c r="F139" s="70" t="s">
+      <c r="F139" s="65" t="s">
         <v>64</v>
       </c>
-      <c r="G139" s="70">
+      <c r="G139" s="65">
         <v>1500</v>
       </c>
-      <c r="H139" s="70" t="s">
+      <c r="H139" s="65" t="s">
         <v>67</v>
       </c>
-      <c r="I139" s="71">
+      <c r="I139" s="66">
         <v>3000</v>
       </c>
-      <c r="J139" s="71" t="s">
+      <c r="J139" s="66" t="s">
         <v>68</v>
       </c>
-      <c r="K139" s="71">
+      <c r="K139" s="66">
         <v>6000</v>
       </c>
-      <c r="L139" s="71" t="s">
+      <c r="L139" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="M139" s="71">
+      <c r="M139" s="66">
         <v>12000</v>
       </c>
-      <c r="N139" s="71" t="s">
+      <c r="N139" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="O139" s="72">
+      <c r="O139" s="67">
         <v>25000</v>
       </c>
-      <c r="P139" s="72" t="s">
+      <c r="P139" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="Q139" s="72">
+      <c r="Q139" s="67">
         <v>50000</v>
       </c>
-      <c r="R139" s="72" t="s">
+      <c r="R139" s="67" t="s">
         <v>88</v>
       </c>
-      <c r="S139" s="46">
+      <c r="S139" s="45">
         <v>100000</v>
       </c>
-      <c r="T139" s="46" t="s">
+      <c r="T139" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="U139" s="73">
+      <c r="U139" s="68">
         <v>250000</v>
       </c>
-      <c r="V139" s="73" t="s">
+      <c r="V139" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="W139" s="74">
+      <c r="W139" s="69">
         <v>500000</v>
       </c>
-      <c r="X139" s="74" t="s">
+      <c r="X139" s="69" t="s">
         <v>70</v>
       </c>
       <c r="Y139" s="4"/>
@@ -9981,54 +9967,74 @@
         <v>48</v>
       </c>
       <c r="B140" t="s">
-        <v>54</v>
-      </c>
-      <c r="C140" s="13">
-        <v>1000000</v>
-      </c>
-      <c r="D140" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="C140" s="9">
+        <v>300</v>
+      </c>
+      <c r="D140" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E140" s="70">
+        <v>750</v>
+      </c>
+      <c r="F140" s="70" t="s">
+        <v>64</v>
+      </c>
+      <c r="G140" s="70">
+        <v>1500</v>
+      </c>
+      <c r="H140" s="70" t="s">
+        <v>67</v>
+      </c>
+      <c r="I140" s="71">
+        <v>3000</v>
+      </c>
+      <c r="J140" s="71" t="s">
+        <v>68</v>
+      </c>
+      <c r="K140" s="71">
+        <v>6000</v>
+      </c>
+      <c r="L140" s="71" t="s">
+        <v>61</v>
+      </c>
+      <c r="M140" s="71">
+        <v>12000</v>
+      </c>
+      <c r="N140" s="71" t="s">
+        <v>66</v>
+      </c>
+      <c r="O140" s="72">
+        <v>25000</v>
+      </c>
+      <c r="P140" s="72" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q140" s="72">
+        <v>50000</v>
+      </c>
+      <c r="R140" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="S140" s="46">
+        <v>100000</v>
+      </c>
+      <c r="T140" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="U140" s="73">
+        <v>250000</v>
+      </c>
+      <c r="V140" s="73" t="s">
         <v>87</v>
       </c>
-      <c r="E140" s="13">
-        <v>1500000</v>
-      </c>
-      <c r="F140" s="13" t="s">
+      <c r="W140" s="74">
+        <v>500000</v>
+      </c>
+      <c r="X140" s="74" t="s">
         <v>70</v>
       </c>
-      <c r="G140" s="13">
-        <v>2000000</v>
-      </c>
-      <c r="H140" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="I140" s="9">
-        <v>3000000</v>
-      </c>
-      <c r="J140" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="K140" s="9">
-        <v>4000000</v>
-      </c>
-      <c r="L140" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="M140" s="9">
-        <v>5000000</v>
-      </c>
-      <c r="N140" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="O140" s="4"/>
-      <c r="P140" s="4"/>
-      <c r="Q140" s="4"/>
-      <c r="R140" s="4"/>
-      <c r="S140" s="4"/>
-      <c r="T140" s="4"/>
-      <c r="U140" s="4"/>
-      <c r="V140" s="4"/>
-      <c r="W140" s="4"/>
-      <c r="X140" s="4"/>
       <c r="Y140" s="4"/>
       <c r="Z140" s="4"/>
       <c r="AA140" s="4"/>
@@ -10043,22 +10049,22 @@
       <c r="B141" t="s">
         <v>54</v>
       </c>
-      <c r="C141" s="11">
+      <c r="C141" s="13">
         <v>1000000</v>
       </c>
-      <c r="D141" s="11" t="s">
+      <c r="D141" s="13" t="s">
         <v>87</v>
       </c>
-      <c r="E141" s="37">
+      <c r="E141" s="13">
         <v>1500000</v>
       </c>
-      <c r="F141" s="37" t="s">
+      <c r="F141" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="G141" s="37">
+      <c r="G141" s="13">
         <v>2000000</v>
       </c>
-      <c r="H141" s="37" t="s">
+      <c r="H141" s="13" t="s">
         <v>77</v>
       </c>
       <c r="I141" s="9">
@@ -10103,40 +10109,40 @@
       <c r="B142" t="s">
         <v>54</v>
       </c>
-      <c r="C142" s="7">
+      <c r="C142" s="11">
         <v>1000000</v>
       </c>
-      <c r="D142" s="7" t="s">
+      <c r="D142" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E142" s="12">
+      <c r="E142" s="37">
         <v>1500000</v>
       </c>
-      <c r="F142" s="12" t="s">
+      <c r="F142" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="G142" s="12">
+      <c r="G142" s="37">
         <v>2000000</v>
       </c>
-      <c r="H142" s="12" t="s">
+      <c r="H142" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="I142" s="8">
+      <c r="I142" s="9">
         <v>3000000</v>
       </c>
-      <c r="J142" s="8" t="s">
+      <c r="J142" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="K142" s="8">
+      <c r="K142" s="9">
         <v>4000000</v>
       </c>
-      <c r="L142" s="8" t="s">
+      <c r="L142" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="M142" s="8">
+      <c r="M142" s="9">
         <v>5000000</v>
       </c>
-      <c r="N142" s="8" t="s">
+      <c r="N142" s="9" t="s">
         <v>73</v>
       </c>
       <c r="O142" s="4"/>
@@ -10163,41 +10169,41 @@
       <c r="B143" t="s">
         <v>54</v>
       </c>
-      <c r="C143" s="79">
-        <v>600000</v>
-      </c>
-      <c r="D143" s="79" t="s">
+      <c r="C143" s="7">
+        <v>1000000</v>
+      </c>
+      <c r="D143" s="7" t="s">
         <v>87</v>
       </c>
-      <c r="E143" s="13">
-        <v>1200000</v>
-      </c>
-      <c r="F143" s="13" t="s">
+      <c r="E143" s="12">
+        <v>1500000</v>
+      </c>
+      <c r="F143" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="G143" s="11">
-        <v>1800000</v>
-      </c>
-      <c r="H143" s="11" t="s">
+      <c r="G143" s="12">
+        <v>2000000</v>
+      </c>
+      <c r="H143" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="I143" s="11">
-        <v>2400000</v>
-      </c>
-      <c r="J143" s="11" t="s">
+      <c r="I143" s="8">
+        <v>3000000</v>
+      </c>
+      <c r="J143" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K143" s="9">
-        <v>3000000</v>
-      </c>
-      <c r="L143" s="9" t="s">
-        <v>58</v>
-      </c>
-      <c r="M143" s="9">
-        <v>3600000</v>
-      </c>
-      <c r="N143" s="9" t="s">
+      <c r="K143" s="8">
+        <v>4000000</v>
+      </c>
+      <c r="L143" s="8" t="s">
         <v>72</v>
+      </c>
+      <c r="M143" s="8">
+        <v>5000000</v>
+      </c>
+      <c r="N143" s="8" t="s">
+        <v>73</v>
       </c>
       <c r="O143" s="4"/>
       <c r="P143" s="4"/>
@@ -10220,18 +10226,45 @@
       <c r="A144" t="s">
         <v>8</v>
       </c>
-      <c r="C144" s="4"/>
-      <c r="D144" s="4"/>
-      <c r="E144" s="4"/>
-      <c r="F144" s="4"/>
-      <c r="G144" s="4"/>
-      <c r="H144" s="4"/>
-      <c r="I144" s="4"/>
-      <c r="J144" s="4"/>
-      <c r="K144" s="4"/>
-      <c r="L144" s="4"/>
-      <c r="M144" s="4"/>
-      <c r="N144" s="4"/>
+      <c r="B144" t="s">
+        <v>54</v>
+      </c>
+      <c r="C144" s="79">
+        <v>600000</v>
+      </c>
+      <c r="D144" s="79" t="s">
+        <v>87</v>
+      </c>
+      <c r="E144" s="13">
+        <v>1200000</v>
+      </c>
+      <c r="F144" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="G144" s="11">
+        <v>1800000</v>
+      </c>
+      <c r="H144" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="I144" s="11">
+        <v>2400000</v>
+      </c>
+      <c r="J144" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="K144" s="9">
+        <v>3000000</v>
+      </c>
+      <c r="L144" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="M144" s="9">
+        <v>3600000</v>
+      </c>
+      <c r="N144" s="9" t="s">
+        <v>72</v>
+      </c>
       <c r="O144" s="4"/>
       <c r="P144" s="4"/>
       <c r="Q144" s="4"/>
@@ -10249,14 +10282,50 @@
       <c r="AC144" s="3"/>
       <c r="AD144" s="3"/>
     </row>
-    <row r="145" spans="27:30" x14ac:dyDescent="0.25">
+    <row r="145" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="C145" s="4"/>
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="G145" s="4"/>
+      <c r="H145" s="4"/>
+      <c r="I145" s="4"/>
+      <c r="J145" s="4"/>
+      <c r="K145" s="4"/>
+      <c r="L145" s="4"/>
+      <c r="M145" s="4"/>
+      <c r="N145" s="4"/>
+      <c r="O145" s="4"/>
+      <c r="P145" s="4"/>
+      <c r="Q145" s="4"/>
+      <c r="R145" s="4"/>
+      <c r="S145" s="4"/>
+      <c r="T145" s="4"/>
+      <c r="U145" s="4"/>
+      <c r="V145" s="4"/>
+      <c r="W145" s="4"/>
+      <c r="X145" s="4"/>
+      <c r="Y145" s="4"/>
+      <c r="Z145" s="4"/>
       <c r="AA145" s="4"/>
       <c r="AB145" s="4"/>
       <c r="AC145" s="3"/>
       <c r="AD145" s="3"/>
     </row>
+    <row r="146" spans="3:30" x14ac:dyDescent="0.25">
+      <c r="AA146" s="4"/>
+      <c r="AB146" s="4"/>
+      <c r="AC146" s="3"/>
+      <c r="AD146" s="3"/>
+    </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
@@ -10264,12 +10333,6 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" fitToHeight="0" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated to include September 2015 update
</commit_message>
<xml_diff>
--- a/ClashOfClans_TechTree/CoC_Spread.xlsx
+++ b/ClashOfClans_TechTree/CoC_Spread.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1293" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1294" uniqueCount="104">
   <si>
     <t>Town Hall</t>
   </si>
@@ -1183,8 +1183,8 @@
   </sheetPr>
   <dimension ref="A1:AD146"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="R17" sqref="R17"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E61" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="O28" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2575,14 +2575,18 @@
       <c r="L26" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="M26" s="7">
+      <c r="M26" s="83">
+        <v>6000000</v>
+      </c>
+      <c r="N26" s="83" t="s">
+        <v>74</v>
+      </c>
+      <c r="O26" s="7">
         <v>8000000</v>
       </c>
-      <c r="N26" s="7" t="s">
+      <c r="P26" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="O26" s="4"/>
-      <c r="P26" s="4"/>
       <c r="Q26" s="4"/>
       <c r="R26" s="4"/>
       <c r="S26" s="4"/>
@@ -10327,12 +10331,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
@@ -10340,11 +10338,17 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:Z1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" fitToHeight="2" orientation="landscape" r:id="rId1"/>
   <headerFooter>
-    <oddFooter>&amp;CVersion 3.0</oddFooter>
+    <oddFooter>&amp;CVersion 3.1</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Of course I forgot to change the training time for lightning,  but that's fixed now
</commit_message>
<xml_diff>
--- a/ClashOfClans_TechTree/CoC_Spread.xlsx
+++ b/ClashOfClans_TechTree/CoC_Spread.xlsx
@@ -1183,8 +1183,8 @@
   </sheetPr>
   <dimension ref="A1:AD146"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="E61" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O28" sqref="O28"/>
+    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A25" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="N26" sqref="N26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2579,7 +2579,7 @@
         <v>6000000</v>
       </c>
       <c r="N26" s="83" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="O26" s="7">
         <v>8000000</v>
@@ -10331,6 +10331,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
     <mergeCell ref="AA1:AB1"/>
     <mergeCell ref="O1:P1"/>
     <mergeCell ref="Q1:R1"/>
@@ -10338,12 +10344,6 @@
     <mergeCell ref="U1:V1"/>
     <mergeCell ref="W1:X1"/>
     <mergeCell ref="Y1:Z1"/>
-    <mergeCell ref="M1:N1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="I1:J1"/>
-    <mergeCell ref="K1:L1"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="45" fitToHeight="2" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Fixed tesla level issue
</commit_message>
<xml_diff>
--- a/ClashOfClans_TechTree/CoC_Spread.xlsx
+++ b/ClashOfClans_TechTree/CoC_Spread.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Work\FMX Docs\CoCSpread\ClashOfClans_TechTree\ClashOfClans_TechTree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/l3g3nd/Git/ClashOfClans_TechTree/ClashOfClans_TechTree/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25596" windowHeight="15924"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460"/>
   </bookViews>
   <sheets>
     <sheet name="Defense and Traps together" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -1018,32 +1018,32 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH175"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="B84" sqref="B84"/>
+    <sheetView tabSelected="1" topLeftCell="A45" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="S119" sqref="S119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="25" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
-    <col min="7" max="7" width="10.77734375" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" customWidth="1"/>
-    <col min="17" max="17" width="10.77734375" customWidth="1"/>
-    <col min="19" max="19" width="10.77734375" customWidth="1"/>
-    <col min="21" max="21" width="10.77734375" customWidth="1"/>
-    <col min="22" max="23" width="10.109375" customWidth="1"/>
-    <col min="25" max="25" width="10.109375" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.83203125" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="23" width="10.1640625" customWidth="1"/>
+    <col min="25" max="25" width="10.1640625" customWidth="1"/>
     <col min="27" max="28" width="10" customWidth="1"/>
-    <col min="29" max="29" width="11.109375" customWidth="1"/>
-    <col min="33" max="33" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.1640625" customWidth="1"/>
+    <col min="33" max="33" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:34" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="25" t="s">
         <v>51</v>
       </c>
@@ -1104,7 +1104,7 @@
       </c>
       <c r="AD1" s="26"/>
     </row>
-    <row r="2" spans="1:34" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:34" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1135,7 +1135,7 @@
       <c r="AC2" s="2"/>
       <c r="AD2" s="2"/>
     </row>
-    <row r="3" spans="1:34" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="25" t="s">
         <v>0</v>
       </c>
@@ -1211,7 +1211,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A4" s="25" t="s">
         <v>4</v>
       </c>
@@ -1271,7 +1271,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A5" s="25" t="s">
         <v>6</v>
       </c>
@@ -1343,7 +1343,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A6" s="25" t="s">
         <v>7</v>
       </c>
@@ -1397,7 +1397,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="25" t="s">
         <v>98</v>
       </c>
@@ -1445,7 +1445,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:34" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:34" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1475,7 +1475,7 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="4"/>
     </row>
-    <row r="9" spans="1:34" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="25" t="s">
         <v>9</v>
       </c>
@@ -1573,7 +1573,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A10" s="25" t="s">
         <v>10</v>
       </c>
@@ -1671,7 +1671,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:34" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:34" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="25" t="s">
         <v>114</v>
       </c>
@@ -1775,7 +1775,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:34" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:34" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="1:34" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:34" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="25" t="s">
         <v>30</v>
       </c>
@@ -1872,7 +1872,7 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="14" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A14" s="25" t="s">
         <v>31</v>
       </c>
@@ -1935,7 +1935,7 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
     </row>
-    <row r="15" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A15" s="25" t="s">
         <v>33</v>
       </c>
@@ -1999,7 +1999,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
     </row>
-    <row r="16" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
         <v>32</v>
       </c>
@@ -2059,7 +2059,7 @@
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
     </row>
-    <row r="17" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
         <v>34</v>
       </c>
@@ -2116,7 +2116,7 @@
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
     </row>
-    <row r="18" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18" s="25" t="s">
         <v>35</v>
       </c>
@@ -2176,7 +2176,7 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
     </row>
-    <row r="19" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19" s="25" t="s">
         <v>36</v>
       </c>
@@ -2236,7 +2236,7 @@
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
     </row>
-    <row r="20" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20" s="25" t="s">
         <v>37</v>
       </c>
@@ -2288,7 +2288,7 @@
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
     </row>
-    <row r="21" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21" s="25" t="s">
         <v>38</v>
       </c>
@@ -2344,7 +2344,7 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22" s="25" t="s">
         <v>39</v>
       </c>
@@ -2400,7 +2400,7 @@
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
     </row>
-    <row r="23" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23" s="25" t="s">
         <v>40</v>
       </c>
@@ -2464,7 +2464,7 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
     </row>
-    <row r="24" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24" s="25" t="s">
         <v>100</v>
       </c>
@@ -2520,7 +2520,7 @@
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
     </row>
-    <row r="25" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25" s="25" t="s">
         <v>41</v>
       </c>
@@ -2570,7 +2570,7 @@
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
     </row>
-    <row r="26" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26" s="25" t="s">
         <v>42</v>
       </c>
@@ -2626,7 +2626,7 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
     </row>
-    <row r="27" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27" s="25" t="s">
         <v>43</v>
       </c>
@@ -2674,7 +2674,7 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
     </row>
-    <row r="28" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="25" t="s">
         <v>44</v>
       </c>
@@ -2722,12 +2722,12 @@
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
     </row>
-    <row r="29" spans="1:30" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:30" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" s="25" t="s">
         <v>90</v>
       </c>
@@ -2791,7 +2791,7 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
     </row>
-    <row r="31" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31" s="25" t="s">
         <v>91</v>
       </c>
@@ -2851,7 +2851,7 @@
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
     </row>
-    <row r="32" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32" s="25" t="s">
         <v>92</v>
       </c>
@@ -2907,7 +2907,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
     </row>
-    <row r="33" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33" s="25" t="s">
         <v>93</v>
       </c>
@@ -2955,7 +2955,7 @@
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
     </row>
-    <row r="34" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34" s="25" t="s">
         <v>94</v>
       </c>
@@ -3011,7 +3011,7 @@
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
     </row>
-    <row r="35" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35" s="25" t="s">
         <v>95</v>
       </c>
@@ -3061,7 +3061,7 @@
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
     </row>
-    <row r="36" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36" s="25" t="s">
         <v>96</v>
       </c>
@@ -3113,7 +3113,7 @@
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
     </row>
-    <row r="37" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="25" t="s">
         <v>97</v>
       </c>
@@ -3165,7 +3165,7 @@
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
     </row>
-    <row r="38" spans="1:30" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:30" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>24</v>
       </c>
@@ -3196,7 +3196,7 @@
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
     </row>
-    <row r="39" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A39" s="25" t="s">
         <v>23</v>
       </c>
@@ -3278,7 +3278,7 @@
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
     </row>
-    <row r="40" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40" s="25" t="s">
         <v>23</v>
       </c>
@@ -3360,7 +3360,7 @@
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
     </row>
-    <row r="41" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41" s="25" t="s">
         <v>23</v>
       </c>
@@ -3442,7 +3442,7 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
     </row>
-    <row r="42" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42" s="25" t="s">
         <v>23</v>
       </c>
@@ -3524,7 +3524,7 @@
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
     </row>
-    <row r="43" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="25" t="s">
         <v>23</v>
       </c>
@@ -3606,7 +3606,7 @@
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
     </row>
-    <row r="44" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="25" t="s">
         <v>23</v>
       </c>
@@ -3688,7 +3688,7 @@
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
     </row>
-    <row r="45" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A45" s="25" t="s">
         <v>23</v>
       </c>
@@ -3770,7 +3770,7 @@
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
     </row>
-    <row r="46" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A46" s="25" t="s">
         <v>46</v>
       </c>
@@ -3852,7 +3852,7 @@
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
     </row>
-    <row r="47" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A47" s="25" t="s">
         <v>46</v>
       </c>
@@ -3936,7 +3936,7 @@
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
     </row>
-    <row r="48" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A48" s="25" t="s">
         <v>46</v>
       </c>
@@ -4020,7 +4020,7 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
     </row>
-    <row r="49" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A49" s="25" t="s">
         <v>46</v>
       </c>
@@ -4104,7 +4104,7 @@
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
     </row>
-    <row r="50" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="25" t="s">
         <v>47</v>
       </c>
@@ -4188,7 +4188,7 @@
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
     </row>
-    <row r="51" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" s="25" t="s">
         <v>47</v>
       </c>
@@ -4272,7 +4272,7 @@
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
     </row>
-    <row r="52" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A52" s="25" t="s">
         <v>47</v>
       </c>
@@ -4356,7 +4356,7 @@
       <c r="AC52" s="3"/>
       <c r="AD52" s="3"/>
     </row>
-    <row r="53" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A53" s="25" t="s">
         <v>47</v>
       </c>
@@ -4440,7 +4440,7 @@
       <c r="AC53" s="3"/>
       <c r="AD53" s="3"/>
     </row>
-    <row r="54" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A54" s="25" t="s">
         <v>47</v>
       </c>
@@ -4524,7 +4524,7 @@
       <c r="AC54" s="3"/>
       <c r="AD54" s="3"/>
     </row>
-    <row r="55" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A55" s="25" t="s">
         <v>47</v>
       </c>
@@ -4608,7 +4608,7 @@
       <c r="AC55" s="3"/>
       <c r="AD55" s="3"/>
     </row>
-    <row r="56" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A56" s="25" t="s">
         <v>47</v>
       </c>
@@ -4692,7 +4692,7 @@
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
     </row>
-    <row r="57" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A57" s="25" t="s">
         <v>48</v>
       </c>
@@ -4776,7 +4776,7 @@
       <c r="AC57" s="3"/>
       <c r="AD57" s="3"/>
     </row>
-    <row r="58" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A58" s="25" t="s">
         <v>48</v>
       </c>
@@ -4860,7 +4860,7 @@
       <c r="AC58" s="3"/>
       <c r="AD58" s="3"/>
     </row>
-    <row r="59" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A59" s="25" t="s">
         <v>48</v>
       </c>
@@ -4944,7 +4944,7 @@
       <c r="AC59" s="3"/>
       <c r="AD59" s="3"/>
     </row>
-    <row r="60" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A60" s="25" t="s">
         <v>48</v>
       </c>
@@ -5028,7 +5028,7 @@
       <c r="AC60" s="3"/>
       <c r="AD60" s="3"/>
     </row>
-    <row r="61" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A61" s="25" t="s">
         <v>49</v>
       </c>
@@ -5088,7 +5088,7 @@
       <c r="AC61" s="3"/>
       <c r="AD61" s="3"/>
     </row>
-    <row r="62" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A62" s="25" t="s">
         <v>49</v>
       </c>
@@ -5148,7 +5148,7 @@
       <c r="AC62" s="3"/>
       <c r="AD62" s="3"/>
     </row>
-    <row r="63" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A63" s="25" t="s">
         <v>49</v>
       </c>
@@ -5208,7 +5208,7 @@
       <c r="AC63" s="3"/>
       <c r="AD63" s="3"/>
     </row>
-    <row r="64" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="25" t="s">
         <v>8</v>
       </c>
@@ -5268,7 +5268,7 @@
       <c r="AC64" s="3"/>
       <c r="AD64" s="3"/>
     </row>
-    <row r="65" spans="1:30" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:30" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>25</v>
       </c>
@@ -5302,7 +5302,7 @@
       <c r="AC65" s="3"/>
       <c r="AD65" s="3"/>
     </row>
-    <row r="66" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A66" s="25" t="s">
         <v>20</v>
       </c>
@@ -5370,7 +5370,7 @@
       <c r="AC66" s="3"/>
       <c r="AD66" s="3"/>
     </row>
-    <row r="67" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A67" s="25" t="s">
         <v>20</v>
       </c>
@@ -5438,7 +5438,7 @@
       <c r="AC67" s="3"/>
       <c r="AD67" s="3"/>
     </row>
-    <row r="68" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A68" s="25" t="s">
         <v>20</v>
       </c>
@@ -5506,7 +5506,7 @@
       <c r="AC68" s="3"/>
       <c r="AD68" s="3"/>
     </row>
-    <row r="69" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A69" s="25" t="s">
         <v>20</v>
       </c>
@@ -5576,7 +5576,7 @@
       <c r="AC69" s="3"/>
       <c r="AD69" s="3"/>
     </row>
-    <row r="70" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A70" s="25" t="s">
         <v>21</v>
       </c>
@@ -5652,7 +5652,7 @@
       <c r="AC70" s="3"/>
       <c r="AD70" s="3"/>
     </row>
-    <row r="71" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A71" s="25" t="s">
         <v>21</v>
       </c>
@@ -5728,7 +5728,7 @@
       <c r="AC71" s="3"/>
       <c r="AD71" s="3"/>
     </row>
-    <row r="72" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A72" s="25" t="s">
         <v>21</v>
       </c>
@@ -5802,7 +5802,7 @@
       <c r="AC72" s="3"/>
       <c r="AD72" s="3"/>
     </row>
-    <row r="73" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A73" s="25" t="s">
         <v>21</v>
       </c>
@@ -5876,7 +5876,7 @@
       <c r="AC73" s="3"/>
       <c r="AD73" s="3"/>
     </row>
-    <row r="74" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A74" s="25" t="s">
         <v>22</v>
       </c>
@@ -5934,7 +5934,7 @@
       <c r="AC74" s="3"/>
       <c r="AD74" s="3"/>
     </row>
-    <row r="75" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="25" t="s">
         <v>22</v>
       </c>
@@ -5992,7 +5992,7 @@
       <c r="AC75" s="3"/>
       <c r="AD75" s="3"/>
     </row>
-    <row r="76" spans="1:30" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:30" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>27</v>
       </c>
@@ -6020,7 +6020,7 @@
       <c r="X76" s="4"/>
       <c r="Y76" s="4"/>
     </row>
-    <row r="77" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A77" s="25" t="s">
         <v>1</v>
       </c>
@@ -6083,7 +6083,7 @@
       <c r="X77" s="4"/>
       <c r="Y77" s="4"/>
     </row>
-    <row r="78" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A78" s="25" t="s">
         <v>1</v>
       </c>
@@ -6145,7 +6145,7 @@
       <c r="X78" s="4"/>
       <c r="Y78" s="4"/>
     </row>
-    <row r="79" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A79" s="25" t="s">
         <v>1</v>
       </c>
@@ -6208,7 +6208,7 @@
       <c r="X79" s="4"/>
       <c r="Y79" s="4"/>
     </row>
-    <row r="80" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A80" s="25" t="s">
         <v>1</v>
       </c>
@@ -6271,7 +6271,7 @@
       <c r="X80" s="4"/>
       <c r="Y80" s="4"/>
     </row>
-    <row r="81" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A81" s="25" t="s">
         <v>88</v>
       </c>
@@ -6326,7 +6326,7 @@
       <c r="X81" s="4"/>
       <c r="Y81" s="4"/>
     </row>
-    <row r="82" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A82" s="25" t="s">
         <v>88</v>
       </c>
@@ -6381,7 +6381,7 @@
       <c r="X82" s="4"/>
       <c r="Y82" s="4"/>
     </row>
-    <row r="83" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A83" s="25" t="s">
         <v>2</v>
       </c>
@@ -6458,7 +6458,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="84" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A84" s="25" t="s">
         <v>2</v>
       </c>
@@ -6535,7 +6535,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="85" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A85" s="25" t="s">
         <v>2</v>
       </c>
@@ -6612,7 +6612,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="86" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A86" s="25" t="s">
         <v>2</v>
       </c>
@@ -6689,7 +6689,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="87" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A87" s="25" t="s">
         <v>2</v>
       </c>
@@ -6766,7 +6766,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="88" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A88" s="25" t="s">
         <v>2</v>
       </c>
@@ -6843,7 +6843,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="89" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A89" s="25" t="s">
         <v>2</v>
       </c>
@@ -6920,7 +6920,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="90" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A90" s="25" t="s">
         <v>2</v>
       </c>
@@ -6997,7 +6997,7 @@
         <v>6500000</v>
       </c>
     </row>
-    <row r="91" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A91" s="25" t="s">
         <v>3</v>
       </c>
@@ -7074,7 +7074,7 @@
         <v>6400000</v>
       </c>
     </row>
-    <row r="92" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A92" s="25" t="s">
         <v>3</v>
       </c>
@@ -7156,7 +7156,7 @@
       <c r="AC92" s="3"/>
       <c r="AD92" s="3"/>
     </row>
-    <row r="93" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A93" s="25" t="s">
         <v>3</v>
       </c>
@@ -7238,7 +7238,7 @@
       <c r="AC93" s="3"/>
       <c r="AD93" s="3"/>
     </row>
-    <row r="94" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A94" s="25" t="s">
         <v>3</v>
       </c>
@@ -7320,7 +7320,7 @@
       <c r="AC94" s="3"/>
       <c r="AD94" s="3"/>
     </row>
-    <row r="95" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A95" s="25" t="s">
         <v>3</v>
       </c>
@@ -7402,7 +7402,7 @@
       <c r="AC95" s="3"/>
       <c r="AD95" s="3"/>
     </row>
-    <row r="96" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A96" s="25" t="s">
         <v>3</v>
       </c>
@@ -7484,7 +7484,7 @@
       <c r="AC96" s="3"/>
       <c r="AD96" s="3"/>
     </row>
-    <row r="97" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A97" s="25" t="s">
         <v>3</v>
       </c>
@@ -7566,7 +7566,7 @@
       <c r="AC97" s="3"/>
       <c r="AD97" s="3"/>
     </row>
-    <row r="98" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A98" s="25" t="s">
         <v>55</v>
       </c>
@@ -7634,7 +7634,7 @@
       <c r="AC98" s="3"/>
       <c r="AD98" s="3"/>
     </row>
-    <row r="99" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A99" s="25" t="s">
         <v>55</v>
       </c>
@@ -7708,7 +7708,7 @@
       <c r="AC99" s="3"/>
       <c r="AD99" s="3"/>
     </row>
-    <row r="100" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A100" s="25" t="s">
         <v>55</v>
       </c>
@@ -7782,7 +7782,7 @@
       <c r="AC100" s="3"/>
       <c r="AD100" s="3"/>
     </row>
-    <row r="101" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A101" s="25" t="s">
         <v>55</v>
       </c>
@@ -7856,7 +7856,7 @@
       <c r="AC101" s="3"/>
       <c r="AD101" s="3"/>
     </row>
-    <row r="102" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A102" s="25" t="s">
         <v>11</v>
       </c>
@@ -7934,7 +7934,7 @@
       <c r="AC102" s="3"/>
       <c r="AD102" s="3"/>
     </row>
-    <row r="103" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A103" s="25" t="s">
         <v>11</v>
       </c>
@@ -8012,7 +8012,7 @@
       <c r="AC103" s="3"/>
       <c r="AD103" s="3"/>
     </row>
-    <row r="104" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A104" s="25" t="s">
         <v>11</v>
       </c>
@@ -8090,7 +8090,7 @@
       <c r="AC104" s="3"/>
       <c r="AD104" s="3"/>
     </row>
-    <row r="105" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A105" s="25" t="s">
         <v>11</v>
       </c>
@@ -8168,7 +8168,7 @@
       <c r="AC105" s="3"/>
       <c r="AD105" s="3"/>
     </row>
-    <row r="106" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A106" s="25" t="s">
         <v>11</v>
       </c>
@@ -8246,7 +8246,7 @@
       <c r="AC106" s="3"/>
       <c r="AD106" s="3"/>
     </row>
-    <row r="107" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A107" s="25" t="s">
         <v>5</v>
       </c>
@@ -8320,7 +8320,7 @@
       <c r="AC107" s="3"/>
       <c r="AD107" s="3"/>
     </row>
-    <row r="108" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A108" s="25" t="s">
         <v>5</v>
       </c>
@@ -8394,7 +8394,7 @@
       <c r="AC108" s="3"/>
       <c r="AD108" s="3"/>
     </row>
-    <row r="109" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A109" s="25" t="s">
         <v>5</v>
       </c>
@@ -8468,53 +8468,53 @@
       <c r="AC109" s="3"/>
       <c r="AD109" s="3"/>
     </row>
-    <row r="110" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A110" s="25" t="s">
         <v>5</v>
       </c>
       <c r="B110" t="s">
         <v>52</v>
       </c>
-      <c r="C110" s="23">
+      <c r="C110" s="22">
         <v>1000000</v>
       </c>
-      <c r="D110" s="23" t="s">
+      <c r="D110" s="22" t="s">
         <v>84</v>
       </c>
-      <c r="E110" s="23">
+      <c r="E110" s="22">
         <v>1250000</v>
       </c>
-      <c r="F110" s="23" t="s">
+      <c r="F110" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="G110" s="23">
+      <c r="G110" s="22">
         <v>1500000</v>
       </c>
-      <c r="H110" s="23" t="s">
+      <c r="H110" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="I110" s="23">
+      <c r="I110" s="22">
         <v>2000000</v>
       </c>
-      <c r="J110" s="23" t="s">
+      <c r="J110" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="K110" s="23">
+      <c r="K110" s="22">
         <v>2500000</v>
       </c>
-      <c r="L110" s="23" t="s">
+      <c r="L110" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="M110" s="23">
+      <c r="M110" s="22">
         <v>3000000</v>
       </c>
-      <c r="N110" s="23" t="s">
+      <c r="N110" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="O110" s="23">
+      <c r="O110" s="22">
         <v>3500000</v>
       </c>
-      <c r="P110" s="23" t="s">
+      <c r="P110" s="22" t="s">
         <v>77</v>
       </c>
       <c r="Q110" s="23">
@@ -8542,7 +8542,7 @@
       <c r="AC110" s="3"/>
       <c r="AD110" s="3"/>
     </row>
-    <row r="111" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A111" s="25" t="s">
         <v>12</v>
       </c>
@@ -8600,7 +8600,7 @@
       <c r="AC111" s="3"/>
       <c r="AD111" s="3"/>
     </row>
-    <row r="112" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A112" s="25" t="s">
         <v>12</v>
       </c>
@@ -8658,7 +8658,7 @@
       <c r="AC112" s="3"/>
       <c r="AD112" s="3"/>
     </row>
-    <row r="113" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A113" s="25" t="s">
         <v>12</v>
       </c>
@@ -8716,7 +8716,7 @@
       <c r="AC113" s="3"/>
       <c r="AD113" s="3"/>
     </row>
-    <row r="114" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A114" s="25" t="s">
         <v>12</v>
       </c>
@@ -8768,7 +8768,7 @@
       <c r="AC114" s="3"/>
       <c r="AD114" s="3"/>
     </row>
-    <row r="115" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A115" s="25" t="s">
         <v>13</v>
       </c>
@@ -8816,7 +8816,7 @@
       <c r="AC115" s="3"/>
       <c r="AD115" s="3"/>
     </row>
-    <row r="116" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A116" s="25" t="s">
         <v>13</v>
       </c>
@@ -8864,7 +8864,7 @@
       <c r="AC116" s="3"/>
       <c r="AD116" s="3"/>
     </row>
-    <row r="117" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A117" s="25" t="s">
         <v>113</v>
       </c>
@@ -8906,7 +8906,7 @@
       <c r="AC117" s="3"/>
       <c r="AD117" s="3"/>
     </row>
-    <row r="118" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A118" s="25" t="s">
         <v>104</v>
       </c>
@@ -8986,7 +8986,7 @@
       <c r="AC118" s="3"/>
       <c r="AD118" s="3"/>
     </row>
-    <row r="119" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A119" s="25" t="s">
         <v>105</v>
       </c>
@@ -9066,7 +9066,7 @@
       <c r="AC119" s="3"/>
       <c r="AD119" s="3"/>
     </row>
-    <row r="120" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A120" s="25" t="s">
         <v>106</v>
       </c>
@@ -9146,7 +9146,7 @@
       <c r="AC120" s="3"/>
       <c r="AD120" s="3"/>
     </row>
-    <row r="121" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A121" s="25" t="s">
         <v>107</v>
       </c>
@@ -9226,7 +9226,7 @@
       <c r="AC121" s="3"/>
       <c r="AD121" s="3"/>
     </row>
-    <row r="122" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A122" s="25" t="s">
         <v>108</v>
       </c>
@@ -9306,7 +9306,7 @@
       <c r="AC122" s="3"/>
       <c r="AD122" s="3"/>
     </row>
-    <row r="123" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A123" s="25" t="s">
         <v>109</v>
       </c>
@@ -9386,7 +9386,7 @@
       <c r="AC123" s="3"/>
       <c r="AD123" s="3"/>
     </row>
-    <row r="124" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A124" s="25" t="s">
         <v>110</v>
       </c>
@@ -9466,7 +9466,7 @@
       <c r="AC124" s="3"/>
       <c r="AD124" s="3"/>
     </row>
-    <row r="125" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A125" s="25" t="s">
         <v>111</v>
       </c>
@@ -9546,7 +9546,7 @@
       <c r="AC125" s="3"/>
       <c r="AD125" s="3"/>
     </row>
-    <row r="126" spans="1:30" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:30" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="25" t="s">
         <v>112</v>
       </c>
@@ -9626,7 +9626,7 @@
       <c r="AC126" s="3"/>
       <c r="AD126" s="3"/>
     </row>
-    <row r="127" spans="1:30" ht="22.2" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:30" ht="23" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>26</v>
       </c>
@@ -9659,7 +9659,7 @@
       <c r="AC127" s="3"/>
       <c r="AD127" s="3"/>
     </row>
-    <row r="128" spans="1:30" ht="15" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:30" ht="16" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A128" s="25" t="s">
         <v>14</v>
       </c>
@@ -9711,7 +9711,7 @@
       <c r="AC128" s="3"/>
       <c r="AD128" s="3"/>
     </row>
-    <row r="129" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A129" s="25" t="s">
         <v>14</v>
       </c>
@@ -9763,7 +9763,7 @@
       <c r="AC129" s="3"/>
       <c r="AD129" s="3"/>
     </row>
-    <row r="130" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A130" s="25" t="s">
         <v>14</v>
       </c>
@@ -9815,7 +9815,7 @@
       <c r="AC130" s="3"/>
       <c r="AD130" s="3"/>
     </row>
-    <row r="131" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A131" s="25" t="s">
         <v>14</v>
       </c>
@@ -9867,7 +9867,7 @@
       <c r="AC131" s="3"/>
       <c r="AD131" s="3"/>
     </row>
-    <row r="132" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A132" s="25" t="s">
         <v>14</v>
       </c>
@@ -9919,7 +9919,7 @@
       <c r="AC132" s="3"/>
       <c r="AD132" s="3"/>
     </row>
-    <row r="133" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A133" s="25" t="s">
         <v>15</v>
       </c>
@@ -9979,7 +9979,7 @@
       <c r="AC133" s="3"/>
       <c r="AD133" s="3"/>
     </row>
-    <row r="134" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A134" s="25" t="s">
         <v>15</v>
       </c>
@@ -10039,7 +10039,7 @@
       <c r="AC134" s="3"/>
       <c r="AD134" s="3"/>
     </row>
-    <row r="135" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A135" s="25" t="s">
         <v>15</v>
       </c>
@@ -10099,7 +10099,7 @@
       <c r="AC135" s="3"/>
       <c r="AD135" s="3"/>
     </row>
-    <row r="136" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A136" s="25" t="s">
         <v>15</v>
       </c>
@@ -10159,7 +10159,7 @@
       <c r="AC136" s="3"/>
       <c r="AD136" s="3"/>
     </row>
-    <row r="137" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A137" s="25" t="s">
         <v>15</v>
       </c>
@@ -10219,7 +10219,7 @@
       <c r="AC137" s="3"/>
       <c r="AD137" s="3"/>
     </row>
-    <row r="138" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A138" s="25" t="s">
         <v>15</v>
       </c>
@@ -10279,7 +10279,7 @@
       <c r="AC138" s="3"/>
       <c r="AD138" s="3"/>
     </row>
-    <row r="139" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A139" s="25" t="s">
         <v>16</v>
       </c>
@@ -10331,7 +10331,7 @@
       <c r="AC139" s="3"/>
       <c r="AD139" s="3"/>
     </row>
-    <row r="140" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A140" s="25" t="s">
         <v>16</v>
       </c>
@@ -10383,7 +10383,7 @@
       <c r="AC140" s="3"/>
       <c r="AD140" s="3"/>
     </row>
-    <row r="141" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A141" s="25" t="s">
         <v>16</v>
       </c>
@@ -10435,7 +10435,7 @@
       <c r="AC141" s="3"/>
       <c r="AD141" s="3"/>
     </row>
-    <row r="142" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A142" s="25" t="s">
         <v>16</v>
       </c>
@@ -10487,7 +10487,7 @@
       <c r="AC142" s="3"/>
       <c r="AD142" s="3"/>
     </row>
-    <row r="143" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A143" s="25" t="s">
         <v>16</v>
       </c>
@@ -10539,7 +10539,7 @@
       <c r="AC143" s="3"/>
       <c r="AD143" s="3"/>
     </row>
-    <row r="144" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A144" s="25" t="s">
         <v>17</v>
       </c>
@@ -10587,7 +10587,7 @@
       <c r="AC144" s="3"/>
       <c r="AD144" s="3"/>
     </row>
-    <row r="145" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A145" s="25" t="s">
         <v>17</v>
       </c>
@@ -10635,7 +10635,7 @@
       <c r="AC145" s="3"/>
       <c r="AD145" s="3"/>
     </row>
-    <row r="146" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A146" s="25" t="s">
         <v>17</v>
       </c>
@@ -10683,7 +10683,7 @@
       <c r="AC146" s="3"/>
       <c r="AD146" s="3"/>
     </row>
-    <row r="147" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A147" s="25" t="s">
         <v>17</v>
       </c>
@@ -10731,7 +10731,7 @@
       <c r="AC147" s="3"/>
       <c r="AD147" s="3"/>
     </row>
-    <row r="148" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A148" s="25" t="s">
         <v>17</v>
       </c>
@@ -10779,7 +10779,7 @@
       <c r="AC148" s="3"/>
       <c r="AD148" s="3"/>
     </row>
-    <row r="149" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A149" s="25" t="s">
         <v>18</v>
       </c>
@@ -10827,7 +10827,7 @@
       <c r="AC149" s="3"/>
       <c r="AD149" s="3"/>
     </row>
-    <row r="150" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A150" s="25" t="s">
         <v>18</v>
       </c>
@@ -10875,7 +10875,7 @@
       <c r="AC150" s="3"/>
       <c r="AD150" s="3"/>
     </row>
-    <row r="151" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A151" s="25" t="s">
         <v>18</v>
       </c>
@@ -10923,7 +10923,7 @@
       <c r="AC151" s="3"/>
       <c r="AD151" s="3"/>
     </row>
-    <row r="152" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A152" s="25" t="s">
         <v>19</v>
       </c>
@@ -10963,7 +10963,7 @@
       <c r="AC152" s="3"/>
       <c r="AD152" s="3"/>
     </row>
-    <row r="153" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A153" s="25" t="s">
         <v>19</v>
       </c>
@@ -11003,7 +11003,7 @@
       <c r="AC153" s="3"/>
       <c r="AD153" s="3"/>
     </row>
-    <row r="154" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A154" s="25" t="s">
         <v>19</v>
       </c>
@@ -11043,7 +11043,7 @@
       <c r="AC154" s="3"/>
       <c r="AD154" s="3"/>
     </row>
-    <row r="155" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A155" s="25" t="s">
         <v>19</v>
       </c>
@@ -11083,7 +11083,7 @@
       <c r="AC155" s="3"/>
       <c r="AD155" s="3"/>
     </row>
-    <row r="156" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A156" s="25" t="s">
         <v>19</v>
       </c>
@@ -11123,7 +11123,7 @@
       <c r="AC156" s="3"/>
       <c r="AD156" s="3"/>
     </row>
-    <row r="157" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A157" s="25" t="s">
         <v>19</v>
       </c>
@@ -11163,7 +11163,7 @@
       <c r="AC157" s="3"/>
       <c r="AD157" s="3"/>
     </row>
-    <row r="158" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:30" x14ac:dyDescent="0.2">
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -11193,119 +11193,119 @@
       <c r="AC158" s="3"/>
       <c r="AD158" s="3"/>
     </row>
-    <row r="159" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:30" x14ac:dyDescent="0.2">
       <c r="Z159" s="4"/>
       <c r="AA159" s="4"/>
       <c r="AB159" s="4"/>
       <c r="AC159" s="3"/>
       <c r="AD159" s="3"/>
     </row>
-    <row r="160" spans="1:30" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:30" x14ac:dyDescent="0.2">
       <c r="Z160" s="4"/>
       <c r="AA160" s="4"/>
       <c r="AB160" s="4"/>
       <c r="AC160" s="3"/>
       <c r="AD160" s="3"/>
     </row>
-    <row r="161" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="161" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z161" s="4"/>
       <c r="AA161" s="4"/>
       <c r="AB161" s="4"/>
       <c r="AC161" s="3"/>
       <c r="AD161" s="3"/>
     </row>
-    <row r="162" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="162" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z162" s="4"/>
       <c r="AA162" s="4"/>
       <c r="AB162" s="4"/>
       <c r="AC162" s="3"/>
       <c r="AD162" s="3"/>
     </row>
-    <row r="163" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="163" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z163" s="4"/>
       <c r="AA163" s="4"/>
       <c r="AB163" s="4"/>
       <c r="AC163" s="3"/>
       <c r="AD163" s="3"/>
     </row>
-    <row r="164" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="164" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z164" s="4"/>
       <c r="AA164" s="4"/>
       <c r="AB164" s="4"/>
       <c r="AC164" s="3"/>
       <c r="AD164" s="3"/>
     </row>
-    <row r="165" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="165" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z165" s="4"/>
       <c r="AA165" s="4"/>
       <c r="AB165" s="4"/>
       <c r="AC165" s="3"/>
       <c r="AD165" s="3"/>
     </row>
-    <row r="166" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="166" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z166" s="4"/>
       <c r="AA166" s="4"/>
       <c r="AB166" s="4"/>
       <c r="AC166" s="3"/>
       <c r="AD166" s="3"/>
     </row>
-    <row r="167" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="167" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z167" s="4"/>
       <c r="AA167" s="4"/>
       <c r="AB167" s="4"/>
       <c r="AC167" s="3"/>
       <c r="AD167" s="3"/>
     </row>
-    <row r="168" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="168" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z168" s="4"/>
       <c r="AA168" s="4"/>
       <c r="AB168" s="4"/>
       <c r="AC168" s="3"/>
       <c r="AD168" s="3"/>
     </row>
-    <row r="169" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="169" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z169" s="4"/>
       <c r="AA169" s="4"/>
       <c r="AB169" s="4"/>
       <c r="AC169" s="3"/>
       <c r="AD169" s="3"/>
     </row>
-    <row r="170" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="170" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z170" s="4"/>
       <c r="AA170" s="4"/>
       <c r="AB170" s="4"/>
       <c r="AC170" s="3"/>
       <c r="AD170" s="3"/>
     </row>
-    <row r="171" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="171" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z171" s="4"/>
       <c r="AA171" s="4"/>
       <c r="AB171" s="4"/>
       <c r="AC171" s="3"/>
       <c r="AD171" s="3"/>
     </row>
-    <row r="172" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="172" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z172" s="4"/>
       <c r="AA172" s="4"/>
       <c r="AB172" s="4"/>
       <c r="AC172" s="3"/>
       <c r="AD172" s="3"/>
     </row>
-    <row r="173" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="173" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z173" s="4"/>
       <c r="AA173" s="4"/>
       <c r="AB173" s="4"/>
       <c r="AC173" s="3"/>
       <c r="AD173" s="3"/>
     </row>
-    <row r="174" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="174" spans="26:30" x14ac:dyDescent="0.2">
       <c r="Z174" s="4"/>
       <c r="AA174" s="4"/>
       <c r="AB174" s="4"/>
       <c r="AC174" s="3"/>
       <c r="AD174" s="3"/>
     </row>
-    <row r="175" spans="26:30" x14ac:dyDescent="0.3">
+    <row r="175" spans="26:30" x14ac:dyDescent="0.2">
       <c r="AA175" s="4"/>
       <c r="AB175" s="4"/>
       <c r="AC175" s="3"/>

</xml_diff>

<commit_message>
fixed formatting for heros
</commit_message>
<xml_diff>
--- a/ClashOfClans_TechTree/CoC_Spread.xlsx
+++ b/ClashOfClans_TechTree/CoC_Spread.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Work\FMX Docs\CoCSpread\ClashOfClans_TechTree\ClashOfClans_TechTree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/l3g3nd/Git/ClashOfClans_TechTree/ClashOfClans_TechTree/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="456" windowWidth="38400" windowHeight="23460"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460"/>
   </bookViews>
   <sheets>
     <sheet name="Defense and Traps together" sheetId="2" r:id="rId1"/>
@@ -17,13 +17,13 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Defense and Traps together'!$1:$2</definedName>
   </definedNames>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -383,7 +383,7 @@
     <t>500,000; 5</t>
   </si>
   <si>
-    <t>5,000; 5</t>
+    <t>+ 5,000 | .5</t>
   </si>
 </sst>
 </file>
@@ -633,7 +633,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="2" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -701,10 +701,13 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1020,97 +1023,97 @@
   <dimension ref="A1:AF175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="AD24" sqref="AD24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16.25" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" customWidth="1"/>
     <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.77734375" customWidth="1"/>
-    <col min="11" max="11" width="10.77734375" customWidth="1"/>
-    <col min="13" max="13" width="10.77734375" customWidth="1"/>
-    <col min="15" max="15" width="10.77734375" customWidth="1"/>
-    <col min="17" max="17" width="10.77734375" customWidth="1"/>
-    <col min="19" max="19" width="10.77734375" customWidth="1"/>
-    <col min="21" max="21" width="10.77734375" customWidth="1"/>
-    <col min="22" max="22" width="10.109375" customWidth="1"/>
-    <col min="23" max="23" width="10.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.109375" customWidth="1"/>
+    <col min="9" max="9" width="10.83203125" customWidth="1"/>
+    <col min="11" max="11" width="10.83203125" customWidth="1"/>
+    <col min="13" max="13" width="10.83203125" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" customWidth="1"/>
+    <col min="19" max="19" width="10.83203125" customWidth="1"/>
+    <col min="21" max="21" width="10.83203125" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" customWidth="1"/>
+    <col min="23" max="23" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="10.1640625" customWidth="1"/>
     <col min="27" max="28" width="10" customWidth="1"/>
-    <col min="29" max="29" width="11.109375" customWidth="1"/>
-    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.1640625" customWidth="1"/>
+    <col min="33" max="33" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:32" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="25">
+      <c r="C1" s="26">
         <v>1</v>
       </c>
-      <c r="D1" s="25"/>
-      <c r="E1" s="25">
+      <c r="D1" s="26"/>
+      <c r="E1" s="26">
         <v>2</v>
       </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25">
+      <c r="F1" s="26"/>
+      <c r="G1" s="26">
         <v>3</v>
       </c>
-      <c r="H1" s="25"/>
-      <c r="I1" s="25">
+      <c r="H1" s="26"/>
+      <c r="I1" s="26">
         <v>4</v>
       </c>
-      <c r="J1" s="25"/>
-      <c r="K1" s="25">
+      <c r="J1" s="26"/>
+      <c r="K1" s="26">
         <v>5</v>
       </c>
-      <c r="L1" s="25"/>
-      <c r="M1" s="25">
+      <c r="L1" s="26"/>
+      <c r="M1" s="26">
         <v>6</v>
       </c>
-      <c r="N1" s="25"/>
-      <c r="O1" s="25">
+      <c r="N1" s="26"/>
+      <c r="O1" s="26">
         <v>7</v>
       </c>
-      <c r="P1" s="25"/>
-      <c r="Q1" s="25">
+      <c r="P1" s="26"/>
+      <c r="Q1" s="26">
         <v>8</v>
       </c>
-      <c r="R1" s="25"/>
-      <c r="S1" s="25">
+      <c r="R1" s="26"/>
+      <c r="S1" s="26">
         <v>9</v>
       </c>
-      <c r="T1" s="25"/>
-      <c r="U1" s="25">
+      <c r="T1" s="26"/>
+      <c r="U1" s="26">
         <v>10</v>
       </c>
-      <c r="V1" s="25"/>
-      <c r="W1" s="25">
+      <c r="V1" s="26"/>
+      <c r="W1" s="26">
         <v>11</v>
       </c>
-      <c r="X1" s="25"/>
-      <c r="Y1" s="25">
+      <c r="X1" s="26"/>
+      <c r="Y1" s="26">
         <v>12</v>
       </c>
-      <c r="Z1" s="25"/>
-      <c r="AA1" s="25">
+      <c r="Z1" s="26"/>
+      <c r="AA1" s="26">
         <v>13</v>
       </c>
-      <c r="AB1" s="25"/>
-      <c r="AC1" s="25">
+      <c r="AB1" s="26"/>
+      <c r="AC1" s="26">
         <v>14</v>
       </c>
-      <c r="AD1" s="25"/>
-      <c r="AE1" s="25">
+      <c r="AD1" s="26"/>
+      <c r="AE1" s="26">
         <v>15</v>
       </c>
-      <c r="AF1" s="25"/>
-    </row>
-    <row r="2" spans="1:32" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="AF1" s="26"/>
+    </row>
+    <row r="2" spans="1:32" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1143,7 +1146,7 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" ht="16.350000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
@@ -1223,7 +1226,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:32" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
@@ -1283,7 +1286,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:32" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
@@ -1355,7 +1358,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:32" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="24" t="s">
         <v>7</v>
       </c>
@@ -1409,7 +1412,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:32" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:32" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="24" t="s">
         <v>98</v>
       </c>
@@ -1457,7 +1460,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:32" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:32" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1487,7 +1490,7 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="4"/>
     </row>
-    <row r="9" spans="1:32" ht="16.350000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:32" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A9" s="24" t="s">
         <v>9</v>
       </c>
@@ -1560,7 +1563,7 @@
       <c r="X9" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="Y9" s="26" t="s">
+      <c r="Y9" s="27" t="s">
         <v>117</v>
       </c>
       <c r="Z9" t="s">
@@ -1572,7 +1575,7 @@
       <c r="AB9" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AC9" s="26" t="s">
+      <c r="AC9" s="27" t="s">
         <v>117</v>
       </c>
       <c r="AD9" t="s">
@@ -1585,7 +1588,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="24" t="s">
         <v>10</v>
       </c>
@@ -1658,7 +1661,7 @@
       <c r="X10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="Y10" s="26" t="s">
+      <c r="Y10" s="27" t="s">
         <v>117</v>
       </c>
       <c r="Z10" t="s">
@@ -1670,7 +1673,7 @@
       <c r="AB10" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AC10" s="26" t="s">
+      <c r="AC10" s="27" t="s">
         <v>117</v>
       </c>
       <c r="AD10" t="s">
@@ -1683,7 +1686,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:32" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="24" t="s">
         <v>113</v>
       </c>
@@ -1702,7 +1705,7 @@
       <c r="F11" s="23" t="s">
         <v>67</v>
       </c>
-      <c r="G11" s="26" t="s">
+      <c r="G11" s="25" t="s">
         <v>116</v>
       </c>
       <c r="H11" t="s">
@@ -1757,7 +1760,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:32" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1790,7 +1793,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="1:32" ht="16.350000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:32" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A13" s="24" t="s">
         <v>30</v>
       </c>
@@ -1854,7 +1857,7 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="14" spans="1:32" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="24" t="s">
         <v>31</v>
       </c>
@@ -1917,7 +1920,7 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
     </row>
-    <row r="15" spans="1:32" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="24" t="s">
         <v>33</v>
       </c>
@@ -1981,7 +1984,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
     </row>
-    <row r="16" spans="1:32" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="24" t="s">
         <v>32</v>
       </c>
@@ -2041,7 +2044,7 @@
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
     </row>
-    <row r="17" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>34</v>
       </c>
@@ -2098,7 +2101,7 @@
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
     </row>
-    <row r="18" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="24" t="s">
         <v>35</v>
       </c>
@@ -2158,7 +2161,7 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
     </row>
-    <row r="19" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="24" t="s">
         <v>36</v>
       </c>
@@ -2218,7 +2221,7 @@
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
     </row>
-    <row r="20" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="24" t="s">
         <v>37</v>
       </c>
@@ -2270,7 +2273,7 @@
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
     </row>
-    <row r="21" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="24" t="s">
         <v>38</v>
       </c>
@@ -2326,7 +2329,7 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="24" t="s">
         <v>39</v>
       </c>
@@ -2382,7 +2385,7 @@
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
     </row>
-    <row r="23" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="24" t="s">
         <v>40</v>
       </c>
@@ -2446,7 +2449,7 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
     </row>
-    <row r="24" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="24" t="s">
         <v>100</v>
       </c>
@@ -2502,7 +2505,7 @@
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
     </row>
-    <row r="25" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="24" t="s">
         <v>41</v>
       </c>
@@ -2552,7 +2555,7 @@
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
     </row>
-    <row r="26" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="24" t="s">
         <v>42</v>
       </c>
@@ -2608,7 +2611,7 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
     </row>
-    <row r="27" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="24" t="s">
         <v>43</v>
       </c>
@@ -2656,7 +2659,7 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
     </row>
-    <row r="28" spans="1:30" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
         <v>44</v>
       </c>
@@ -2704,12 +2707,12 @@
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
     </row>
-    <row r="29" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A30" s="24" t="s">
         <v>90</v>
       </c>
@@ -2773,7 +2776,7 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
     </row>
-    <row r="31" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="24" t="s">
         <v>91</v>
       </c>
@@ -2833,7 +2836,7 @@
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
     </row>
-    <row r="32" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="24" t="s">
         <v>92</v>
       </c>
@@ -2889,7 +2892,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
     </row>
-    <row r="33" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="24" t="s">
         <v>93</v>
       </c>
@@ -2937,7 +2940,7 @@
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
     </row>
-    <row r="34" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="24" t="s">
         <v>94</v>
       </c>
@@ -2993,7 +2996,7 @@
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
     </row>
-    <row r="35" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="24" t="s">
         <v>95</v>
       </c>
@@ -3043,7 +3046,7 @@
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
     </row>
-    <row r="36" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="24" t="s">
         <v>96</v>
       </c>
@@ -3095,7 +3098,7 @@
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
     </row>
-    <row r="37" spans="1:30" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
         <v>97</v>
       </c>
@@ -3147,7 +3150,7 @@
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
     </row>
-    <row r="38" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
         <v>24</v>
       </c>
@@ -3178,7 +3181,7 @@
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
     </row>
-    <row r="39" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A39" s="24" t="s">
         <v>23</v>
       </c>
@@ -3260,7 +3263,7 @@
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
     </row>
-    <row r="40" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="24" t="s">
         <v>23</v>
       </c>
@@ -3342,7 +3345,7 @@
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
     </row>
-    <row r="41" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="24" t="s">
         <v>23</v>
       </c>
@@ -3424,7 +3427,7 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
     </row>
-    <row r="42" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="24" t="s">
         <v>23</v>
       </c>
@@ -3506,7 +3509,7 @@
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
     </row>
-    <row r="43" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="24" t="s">
         <v>23</v>
       </c>
@@ -3588,7 +3591,7 @@
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
     </row>
-    <row r="44" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="24" t="s">
         <v>23</v>
       </c>
@@ -3670,7 +3673,7 @@
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
     </row>
-    <row r="45" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="24" t="s">
         <v>23</v>
       </c>
@@ -3752,7 +3755,7 @@
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
     </row>
-    <row r="46" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="24" t="s">
         <v>46</v>
       </c>
@@ -3834,7 +3837,7 @@
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
     </row>
-    <row r="47" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="24" t="s">
         <v>46</v>
       </c>
@@ -3918,7 +3921,7 @@
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
     </row>
-    <row r="48" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="24" t="s">
         <v>46</v>
       </c>
@@ -4002,7 +4005,7 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
     </row>
-    <row r="49" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
         <v>46</v>
       </c>
@@ -4086,7 +4089,7 @@
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
     </row>
-    <row r="50" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="24" t="s">
         <v>47</v>
       </c>
@@ -4170,7 +4173,7 @@
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
     </row>
-    <row r="51" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="24" t="s">
         <v>47</v>
       </c>
@@ -4254,7 +4257,7 @@
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
     </row>
-    <row r="52" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="24" t="s">
         <v>47</v>
       </c>
@@ -4338,7 +4341,7 @@
       <c r="AC52" s="3"/>
       <c r="AD52" s="3"/>
     </row>
-    <row r="53" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="24" t="s">
         <v>47</v>
       </c>
@@ -4422,7 +4425,7 @@
       <c r="AC53" s="3"/>
       <c r="AD53" s="3"/>
     </row>
-    <row r="54" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="24" t="s">
         <v>47</v>
       </c>
@@ -4506,7 +4509,7 @@
       <c r="AC54" s="3"/>
       <c r="AD54" s="3"/>
     </row>
-    <row r="55" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="24" t="s">
         <v>47</v>
       </c>
@@ -4590,7 +4593,7 @@
       <c r="AC55" s="3"/>
       <c r="AD55" s="3"/>
     </row>
-    <row r="56" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="24" t="s">
         <v>47</v>
       </c>
@@ -4674,7 +4677,7 @@
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
     </row>
-    <row r="57" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="24" t="s">
         <v>48</v>
       </c>
@@ -4758,7 +4761,7 @@
       <c r="AC57" s="3"/>
       <c r="AD57" s="3"/>
     </row>
-    <row r="58" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="24" t="s">
         <v>48</v>
       </c>
@@ -4842,7 +4845,7 @@
       <c r="AC58" s="3"/>
       <c r="AD58" s="3"/>
     </row>
-    <row r="59" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="24" t="s">
         <v>48</v>
       </c>
@@ -4926,7 +4929,7 @@
       <c r="AC59" s="3"/>
       <c r="AD59" s="3"/>
     </row>
-    <row r="60" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="24" t="s">
         <v>48</v>
       </c>
@@ -5010,7 +5013,7 @@
       <c r="AC60" s="3"/>
       <c r="AD60" s="3"/>
     </row>
-    <row r="61" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="24" t="s">
         <v>49</v>
       </c>
@@ -5070,7 +5073,7 @@
       <c r="AC61" s="3"/>
       <c r="AD61" s="3"/>
     </row>
-    <row r="62" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="24" t="s">
         <v>49</v>
       </c>
@@ -5130,7 +5133,7 @@
       <c r="AC62" s="3"/>
       <c r="AD62" s="3"/>
     </row>
-    <row r="63" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="24" t="s">
         <v>49</v>
       </c>
@@ -5190,7 +5193,7 @@
       <c r="AC63" s="3"/>
       <c r="AD63" s="3"/>
     </row>
-    <row r="64" spans="1:30" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A64" s="24" t="s">
         <v>8</v>
       </c>
@@ -5250,7 +5253,7 @@
       <c r="AC64" s="3"/>
       <c r="AD64" s="3"/>
     </row>
-    <row r="65" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A65" s="1" t="s">
         <v>25</v>
       </c>
@@ -5284,7 +5287,7 @@
       <c r="AC65" s="3"/>
       <c r="AD65" s="3"/>
     </row>
-    <row r="66" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A66" s="24" t="s">
         <v>20</v>
       </c>
@@ -5352,7 +5355,7 @@
       <c r="AC66" s="3"/>
       <c r="AD66" s="3"/>
     </row>
-    <row r="67" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A67" s="24" t="s">
         <v>20</v>
       </c>
@@ -5420,7 +5423,7 @@
       <c r="AC67" s="3"/>
       <c r="AD67" s="3"/>
     </row>
-    <row r="68" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A68" s="24" t="s">
         <v>20</v>
       </c>
@@ -5488,7 +5491,7 @@
       <c r="AC68" s="3"/>
       <c r="AD68" s="3"/>
     </row>
-    <row r="69" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A69" s="24" t="s">
         <v>20</v>
       </c>
@@ -5558,7 +5561,7 @@
       <c r="AC69" s="3"/>
       <c r="AD69" s="3"/>
     </row>
-    <row r="70" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="24" t="s">
         <v>21</v>
       </c>
@@ -5634,7 +5637,7 @@
       <c r="AC70" s="3"/>
       <c r="AD70" s="3"/>
     </row>
-    <row r="71" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="24" t="s">
         <v>21</v>
       </c>
@@ -5710,7 +5713,7 @@
       <c r="AC71" s="3"/>
       <c r="AD71" s="3"/>
     </row>
-    <row r="72" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="24" t="s">
         <v>21</v>
       </c>
@@ -5784,7 +5787,7 @@
       <c r="AC72" s="3"/>
       <c r="AD72" s="3"/>
     </row>
-    <row r="73" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="24" t="s">
         <v>21</v>
       </c>
@@ -5858,7 +5861,7 @@
       <c r="AC73" s="3"/>
       <c r="AD73" s="3"/>
     </row>
-    <row r="74" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="24" t="s">
         <v>22</v>
       </c>
@@ -5916,7 +5919,7 @@
       <c r="AC74" s="3"/>
       <c r="AD74" s="3"/>
     </row>
-    <row r="75" spans="1:30" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="24" t="s">
         <v>22</v>
       </c>
@@ -5974,7 +5977,7 @@
       <c r="AC75" s="3"/>
       <c r="AD75" s="3"/>
     </row>
-    <row r="76" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="1" t="s">
         <v>27</v>
       </c>
@@ -6002,7 +6005,7 @@
       <c r="X76" s="4"/>
       <c r="Y76" s="4"/>
     </row>
-    <row r="77" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A77" s="24" t="s">
         <v>1</v>
       </c>
@@ -6065,7 +6068,7 @@
       <c r="X77" s="4"/>
       <c r="Y77" s="4"/>
     </row>
-    <row r="78" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A78" s="24" t="s">
         <v>1</v>
       </c>
@@ -6127,7 +6130,7 @@
       <c r="X78" s="4"/>
       <c r="Y78" s="4"/>
     </row>
-    <row r="79" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A79" s="24" t="s">
         <v>1</v>
       </c>
@@ -6190,7 +6193,7 @@
       <c r="X79" s="4"/>
       <c r="Y79" s="4"/>
     </row>
-    <row r="80" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A80" s="24" t="s">
         <v>1</v>
       </c>
@@ -6253,7 +6256,7 @@
       <c r="X80" s="4"/>
       <c r="Y80" s="4"/>
     </row>
-    <row r="81" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A81" s="24" t="s">
         <v>88</v>
       </c>
@@ -6308,7 +6311,7 @@
       <c r="X81" s="4"/>
       <c r="Y81" s="4"/>
     </row>
-    <row r="82" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A82" s="24" t="s">
         <v>88</v>
       </c>
@@ -6363,7 +6366,7 @@
       <c r="X82" s="4"/>
       <c r="Y82" s="4"/>
     </row>
-    <row r="83" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A83" s="24" t="s">
         <v>2</v>
       </c>
@@ -6449,7 +6452,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A84" s="24" t="s">
         <v>2</v>
       </c>
@@ -6535,7 +6538,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A85" s="24" t="s">
         <v>2</v>
       </c>
@@ -6621,7 +6624,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A86" s="24" t="s">
         <v>2</v>
       </c>
@@ -6707,7 +6710,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A87" s="24" t="s">
         <v>2</v>
       </c>
@@ -6793,7 +6796,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A88" s="24" t="s">
         <v>2</v>
       </c>
@@ -6879,7 +6882,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A89" s="24" t="s">
         <v>2</v>
       </c>
@@ -6965,7 +6968,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A90" s="24" t="s">
         <v>2</v>
       </c>
@@ -7051,7 +7054,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A91" s="24" t="s">
         <v>3</v>
       </c>
@@ -7137,7 +7140,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A92" s="24" t="s">
         <v>3</v>
       </c>
@@ -7225,7 +7228,7 @@
       <c r="AC92" s="3"/>
       <c r="AD92" s="3"/>
     </row>
-    <row r="93" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A93" s="24" t="s">
         <v>3</v>
       </c>
@@ -7313,7 +7316,7 @@
       <c r="AC93" s="3"/>
       <c r="AD93" s="3"/>
     </row>
-    <row r="94" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A94" s="24" t="s">
         <v>3</v>
       </c>
@@ -7401,7 +7404,7 @@
       <c r="AC94" s="3"/>
       <c r="AD94" s="3"/>
     </row>
-    <row r="95" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A95" s="24" t="s">
         <v>3</v>
       </c>
@@ -7489,7 +7492,7 @@
       <c r="AC95" s="3"/>
       <c r="AD95" s="3"/>
     </row>
-    <row r="96" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A96" s="24" t="s">
         <v>3</v>
       </c>
@@ -7577,7 +7580,7 @@
       <c r="AC96" s="3"/>
       <c r="AD96" s="3"/>
     </row>
-    <row r="97" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A97" s="24" t="s">
         <v>3</v>
       </c>
@@ -7665,7 +7668,7 @@
       <c r="AC97" s="3"/>
       <c r="AD97" s="3"/>
     </row>
-    <row r="98" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A98" s="24" t="s">
         <v>55</v>
       </c>
@@ -7733,7 +7736,7 @@
       <c r="AC98" s="3"/>
       <c r="AD98" s="3"/>
     </row>
-    <row r="99" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A99" s="24" t="s">
         <v>55</v>
       </c>
@@ -7798,7 +7801,7 @@
       <c r="AC99" s="3"/>
       <c r="AD99" s="3"/>
     </row>
-    <row r="100" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A100" s="24" t="s">
         <v>55</v>
       </c>
@@ -7863,7 +7866,7 @@
       <c r="AC100" s="3"/>
       <c r="AD100" s="3"/>
     </row>
-    <row r="101" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A101" s="24" t="s">
         <v>55</v>
       </c>
@@ -7928,7 +7931,7 @@
       <c r="AC101" s="3"/>
       <c r="AD101" s="3"/>
     </row>
-    <row r="102" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="24" t="s">
         <v>11</v>
       </c>
@@ -7997,7 +8000,7 @@
       <c r="AC102" s="3"/>
       <c r="AD102" s="3"/>
     </row>
-    <row r="103" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A103" s="24" t="s">
         <v>11</v>
       </c>
@@ -8066,7 +8069,7 @@
       <c r="AC103" s="3"/>
       <c r="AD103" s="3"/>
     </row>
-    <row r="104" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A104" s="24" t="s">
         <v>11</v>
       </c>
@@ -8135,7 +8138,7 @@
       <c r="AC104" s="3"/>
       <c r="AD104" s="3"/>
     </row>
-    <row r="105" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A105" s="24" t="s">
         <v>11</v>
       </c>
@@ -8204,7 +8207,7 @@
       <c r="AC105" s="3"/>
       <c r="AD105" s="3"/>
     </row>
-    <row r="106" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A106" s="24" t="s">
         <v>11</v>
       </c>
@@ -8273,7 +8276,7 @@
       <c r="AC106" s="3"/>
       <c r="AD106" s="3"/>
     </row>
-    <row r="107" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A107" s="24" t="s">
         <v>5</v>
       </c>
@@ -8338,7 +8341,7 @@
       <c r="AC107" s="3"/>
       <c r="AD107" s="3"/>
     </row>
-    <row r="108" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A108" s="24" t="s">
         <v>5</v>
       </c>
@@ -8403,7 +8406,7 @@
       <c r="AC108" s="3"/>
       <c r="AD108" s="3"/>
     </row>
-    <row r="109" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A109" s="24" t="s">
         <v>5</v>
       </c>
@@ -8468,7 +8471,7 @@
       <c r="AC109" s="3"/>
       <c r="AD109" s="3"/>
     </row>
-    <row r="110" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A110" s="24" t="s">
         <v>5</v>
       </c>
@@ -8533,7 +8536,7 @@
       <c r="AC110" s="3"/>
       <c r="AD110" s="3"/>
     </row>
-    <row r="111" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A111" s="24" t="s">
         <v>12</v>
       </c>
@@ -8582,7 +8585,7 @@
       <c r="AC111" s="3"/>
       <c r="AD111" s="3"/>
     </row>
-    <row r="112" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A112" s="24" t="s">
         <v>12</v>
       </c>
@@ -8631,7 +8634,7 @@
       <c r="AC112" s="3"/>
       <c r="AD112" s="3"/>
     </row>
-    <row r="113" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A113" s="24" t="s">
         <v>12</v>
       </c>
@@ -8680,7 +8683,7 @@
       <c r="AC113" s="3"/>
       <c r="AD113" s="3"/>
     </row>
-    <row r="114" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A114" s="24" t="s">
         <v>12</v>
       </c>
@@ -8732,7 +8735,7 @@
       <c r="AC114" s="3"/>
       <c r="AD114" s="3"/>
     </row>
-    <row r="115" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A115" s="24" t="s">
         <v>13</v>
       </c>
@@ -8780,7 +8783,7 @@
       <c r="AC115" s="3"/>
       <c r="AD115" s="3"/>
     </row>
-    <row r="116" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A116" s="24" t="s">
         <v>13</v>
       </c>
@@ -8828,7 +8831,7 @@
       <c r="AC116" s="3"/>
       <c r="AD116" s="3"/>
     </row>
-    <row r="117" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A117" s="24" t="s">
         <v>112</v>
       </c>
@@ -8870,7 +8873,7 @@
       <c r="AC117" s="3"/>
       <c r="AD117" s="3"/>
     </row>
-    <row r="118" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A118" s="24" t="s">
         <v>103</v>
       </c>
@@ -8950,7 +8953,7 @@
       <c r="AC118" s="3"/>
       <c r="AD118" s="3"/>
     </row>
-    <row r="119" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A119" s="24" t="s">
         <v>104</v>
       </c>
@@ -9030,7 +9033,7 @@
       <c r="AC119" s="3"/>
       <c r="AD119" s="3"/>
     </row>
-    <row r="120" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A120" s="24" t="s">
         <v>105</v>
       </c>
@@ -9110,7 +9113,7 @@
       <c r="AC120" s="3"/>
       <c r="AD120" s="3"/>
     </row>
-    <row r="121" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A121" s="24" t="s">
         <v>106</v>
       </c>
@@ -9190,7 +9193,7 @@
       <c r="AC121" s="3"/>
       <c r="AD121" s="3"/>
     </row>
-    <row r="122" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A122" s="24" t="s">
         <v>107</v>
       </c>
@@ -9270,7 +9273,7 @@
       <c r="AC122" s="3"/>
       <c r="AD122" s="3"/>
     </row>
-    <row r="123" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A123" s="24" t="s">
         <v>108</v>
       </c>
@@ -9350,7 +9353,7 @@
       <c r="AC123" s="3"/>
       <c r="AD123" s="3"/>
     </row>
-    <row r="124" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A124" s="24" t="s">
         <v>109</v>
       </c>
@@ -9430,7 +9433,7 @@
       <c r="AC124" s="3"/>
       <c r="AD124" s="3"/>
     </row>
-    <row r="125" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A125" s="24" t="s">
         <v>110</v>
       </c>
@@ -9510,7 +9513,7 @@
       <c r="AC125" s="3"/>
       <c r="AD125" s="3"/>
     </row>
-    <row r="126" spans="1:30" ht="16.350000000000001" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A126" s="24" t="s">
         <v>111</v>
       </c>
@@ -9590,7 +9593,7 @@
       <c r="AC126" s="3"/>
       <c r="AD126" s="3"/>
     </row>
-    <row r="127" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A127" s="1" t="s">
         <v>26</v>
       </c>
@@ -9623,7 +9626,7 @@
       <c r="AC127" s="3"/>
       <c r="AD127" s="3"/>
     </row>
-    <row r="128" spans="1:30" ht="16.350000000000001" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A128" s="24" t="s">
         <v>14</v>
       </c>
@@ -9675,7 +9678,7 @@
       <c r="AC128" s="3"/>
       <c r="AD128" s="3"/>
     </row>
-    <row r="129" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A129" s="24" t="s">
         <v>14</v>
       </c>
@@ -9727,7 +9730,7 @@
       <c r="AC129" s="3"/>
       <c r="AD129" s="3"/>
     </row>
-    <row r="130" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A130" s="24" t="s">
         <v>14</v>
       </c>
@@ -9779,7 +9782,7 @@
       <c r="AC130" s="3"/>
       <c r="AD130" s="3"/>
     </row>
-    <row r="131" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A131" s="24" t="s">
         <v>14</v>
       </c>
@@ -9831,7 +9834,7 @@
       <c r="AC131" s="3"/>
       <c r="AD131" s="3"/>
     </row>
-    <row r="132" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A132" s="24" t="s">
         <v>14</v>
       </c>
@@ -9883,7 +9886,7 @@
       <c r="AC132" s="3"/>
       <c r="AD132" s="3"/>
     </row>
-    <row r="133" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A133" s="24" t="s">
         <v>15</v>
       </c>
@@ -9943,7 +9946,7 @@
       <c r="AC133" s="3"/>
       <c r="AD133" s="3"/>
     </row>
-    <row r="134" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A134" s="24" t="s">
         <v>15</v>
       </c>
@@ -10003,7 +10006,7 @@
       <c r="AC134" s="3"/>
       <c r="AD134" s="3"/>
     </row>
-    <row r="135" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A135" s="24" t="s">
         <v>15</v>
       </c>
@@ -10063,7 +10066,7 @@
       <c r="AC135" s="3"/>
       <c r="AD135" s="3"/>
     </row>
-    <row r="136" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A136" s="24" t="s">
         <v>15</v>
       </c>
@@ -10123,7 +10126,7 @@
       <c r="AC136" s="3"/>
       <c r="AD136" s="3"/>
     </row>
-    <row r="137" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="24" t="s">
         <v>15</v>
       </c>
@@ -10183,7 +10186,7 @@
       <c r="AC137" s="3"/>
       <c r="AD137" s="3"/>
     </row>
-    <row r="138" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A138" s="24" t="s">
         <v>15</v>
       </c>
@@ -10243,7 +10246,7 @@
       <c r="AC138" s="3"/>
       <c r="AD138" s="3"/>
     </row>
-    <row r="139" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A139" s="24" t="s">
         <v>16</v>
       </c>
@@ -10295,7 +10298,7 @@
       <c r="AC139" s="3"/>
       <c r="AD139" s="3"/>
     </row>
-    <row r="140" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A140" s="24" t="s">
         <v>16</v>
       </c>
@@ -10347,7 +10350,7 @@
       <c r="AC140" s="3"/>
       <c r="AD140" s="3"/>
     </row>
-    <row r="141" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A141" s="24" t="s">
         <v>16</v>
       </c>
@@ -10399,7 +10402,7 @@
       <c r="AC141" s="3"/>
       <c r="AD141" s="3"/>
     </row>
-    <row r="142" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A142" s="24" t="s">
         <v>16</v>
       </c>
@@ -10451,7 +10454,7 @@
       <c r="AC142" s="3"/>
       <c r="AD142" s="3"/>
     </row>
-    <row r="143" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A143" s="24" t="s">
         <v>16</v>
       </c>
@@ -10503,7 +10506,7 @@
       <c r="AC143" s="3"/>
       <c r="AD143" s="3"/>
     </row>
-    <row r="144" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A144" s="24" t="s">
         <v>17</v>
       </c>
@@ -10551,7 +10554,7 @@
       <c r="AC144" s="3"/>
       <c r="AD144" s="3"/>
     </row>
-    <row r="145" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A145" s="24" t="s">
         <v>17</v>
       </c>
@@ -10599,7 +10602,7 @@
       <c r="AC145" s="3"/>
       <c r="AD145" s="3"/>
     </row>
-    <row r="146" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A146" s="24" t="s">
         <v>17</v>
       </c>
@@ -10647,7 +10650,7 @@
       <c r="AC146" s="3"/>
       <c r="AD146" s="3"/>
     </row>
-    <row r="147" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A147" s="24" t="s">
         <v>17</v>
       </c>
@@ -10695,7 +10698,7 @@
       <c r="AC147" s="3"/>
       <c r="AD147" s="3"/>
     </row>
-    <row r="148" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A148" s="24" t="s">
         <v>17</v>
       </c>
@@ -10743,7 +10746,7 @@
       <c r="AC148" s="3"/>
       <c r="AD148" s="3"/>
     </row>
-    <row r="149" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A149" s="24" t="s">
         <v>18</v>
       </c>
@@ -10791,7 +10794,7 @@
       <c r="AC149" s="3"/>
       <c r="AD149" s="3"/>
     </row>
-    <row r="150" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A150" s="24" t="s">
         <v>18</v>
       </c>
@@ -10839,7 +10842,7 @@
       <c r="AC150" s="3"/>
       <c r="AD150" s="3"/>
     </row>
-    <row r="151" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A151" s="24" t="s">
         <v>18</v>
       </c>
@@ -10887,7 +10890,7 @@
       <c r="AC151" s="3"/>
       <c r="AD151" s="3"/>
     </row>
-    <row r="152" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A152" s="24" t="s">
         <v>19</v>
       </c>
@@ -10927,7 +10930,7 @@
       <c r="AC152" s="3"/>
       <c r="AD152" s="3"/>
     </row>
-    <row r="153" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A153" s="24" t="s">
         <v>19</v>
       </c>
@@ -10967,7 +10970,7 @@
       <c r="AC153" s="3"/>
       <c r="AD153" s="3"/>
     </row>
-    <row r="154" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A154" s="24" t="s">
         <v>19</v>
       </c>
@@ -11007,7 +11010,7 @@
       <c r="AC154" s="3"/>
       <c r="AD154" s="3"/>
     </row>
-    <row r="155" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A155" s="24" t="s">
         <v>19</v>
       </c>
@@ -11047,7 +11050,7 @@
       <c r="AC155" s="3"/>
       <c r="AD155" s="3"/>
     </row>
-    <row r="156" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A156" s="24" t="s">
         <v>19</v>
       </c>
@@ -11087,7 +11090,7 @@
       <c r="AC156" s="3"/>
       <c r="AD156" s="3"/>
     </row>
-    <row r="157" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A157" s="24" t="s">
         <v>19</v>
       </c>
@@ -11127,7 +11130,7 @@
       <c r="AC157" s="3"/>
       <c r="AD157" s="3"/>
     </row>
-    <row r="158" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -11157,119 +11160,119 @@
       <c r="AC158" s="3"/>
       <c r="AD158" s="3"/>
     </row>
-    <row r="159" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z159" s="4"/>
       <c r="AA159" s="4"/>
       <c r="AB159" s="4"/>
       <c r="AC159" s="3"/>
       <c r="AD159" s="3"/>
     </row>
-    <row r="160" spans="1:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z160" s="4"/>
       <c r="AA160" s="4"/>
       <c r="AB160" s="4"/>
       <c r="AC160" s="3"/>
       <c r="AD160" s="3"/>
     </row>
-    <row r="161" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="161" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z161" s="4"/>
       <c r="AA161" s="4"/>
       <c r="AB161" s="4"/>
       <c r="AC161" s="3"/>
       <c r="AD161" s="3"/>
     </row>
-    <row r="162" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="162" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z162" s="4"/>
       <c r="AA162" s="4"/>
       <c r="AB162" s="4"/>
       <c r="AC162" s="3"/>
       <c r="AD162" s="3"/>
     </row>
-    <row r="163" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="163" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z163" s="4"/>
       <c r="AA163" s="4"/>
       <c r="AB163" s="4"/>
       <c r="AC163" s="3"/>
       <c r="AD163" s="3"/>
     </row>
-    <row r="164" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="164" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z164" s="4"/>
       <c r="AA164" s="4"/>
       <c r="AB164" s="4"/>
       <c r="AC164" s="3"/>
       <c r="AD164" s="3"/>
     </row>
-    <row r="165" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="165" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z165" s="4"/>
       <c r="AA165" s="4"/>
       <c r="AB165" s="4"/>
       <c r="AC165" s="3"/>
       <c r="AD165" s="3"/>
     </row>
-    <row r="166" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="166" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z166" s="4"/>
       <c r="AA166" s="4"/>
       <c r="AB166" s="4"/>
       <c r="AC166" s="3"/>
       <c r="AD166" s="3"/>
     </row>
-    <row r="167" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="167" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z167" s="4"/>
       <c r="AA167" s="4"/>
       <c r="AB167" s="4"/>
       <c r="AC167" s="3"/>
       <c r="AD167" s="3"/>
     </row>
-    <row r="168" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="168" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z168" s="4"/>
       <c r="AA168" s="4"/>
       <c r="AB168" s="4"/>
       <c r="AC168" s="3"/>
       <c r="AD168" s="3"/>
     </row>
-    <row r="169" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="169" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z169" s="4"/>
       <c r="AA169" s="4"/>
       <c r="AB169" s="4"/>
       <c r="AC169" s="3"/>
       <c r="AD169" s="3"/>
     </row>
-    <row r="170" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="170" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z170" s="4"/>
       <c r="AA170" s="4"/>
       <c r="AB170" s="4"/>
       <c r="AC170" s="3"/>
       <c r="AD170" s="3"/>
     </row>
-    <row r="171" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="171" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z171" s="4"/>
       <c r="AA171" s="4"/>
       <c r="AB171" s="4"/>
       <c r="AC171" s="3"/>
       <c r="AD171" s="3"/>
     </row>
-    <row r="172" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="172" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z172" s="4"/>
       <c r="AA172" s="4"/>
       <c r="AB172" s="4"/>
       <c r="AC172" s="3"/>
       <c r="AD172" s="3"/>
     </row>
-    <row r="173" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="173" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z173" s="4"/>
       <c r="AA173" s="4"/>
       <c r="AB173" s="4"/>
       <c r="AC173" s="3"/>
       <c r="AD173" s="3"/>
     </row>
-    <row r="174" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="174" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="Z174" s="4"/>
       <c r="AA174" s="4"/>
       <c r="AB174" s="4"/>
       <c r="AC174" s="3"/>
       <c r="AD174" s="3"/>
     </row>
-    <row r="175" spans="26:30" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="175" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="AA175" s="4"/>
       <c r="AB175" s="4"/>
       <c r="AC175" s="3"/>

</xml_diff>

<commit_message>
Grand Warden Format Fix
Passed on hero formatting for warden.
</commit_message>
<xml_diff>
--- a/ClashOfClans_TechTree/CoC_Spread.xlsx
+++ b/ClashOfClans_TechTree/CoC_Spread.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26606"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/l3g3nd/Git/ClashOfClans_TechTree/ClashOfClans_TechTree/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_Work\FMX Docs\CoCSpread\ClashOfClans_TechTree\ClashOfClans_TechTree\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="23460"/>
+    <workbookView xWindow="0" yWindow="456" windowWidth="38400" windowHeight="23460"/>
   </bookViews>
   <sheets>
     <sheet name="Defense and Traps together" sheetId="2" r:id="rId1"/>
@@ -19,11 +19,11 @@
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
-    </ext>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
 </workbook>
@@ -380,10 +380,10 @@
     <t>Level 13</t>
   </si>
   <si>
-    <t>500,000; 5</t>
-  </si>
-  <si>
     <t>+ 5,000 | .5</t>
+  </si>
+  <si>
+    <t>500,000 | .5</t>
   </si>
 </sst>
 </file>
@@ -704,10 +704,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="4" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1023,97 +1023,97 @@
   <dimension ref="A1:AF175"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="AD24" sqref="AD24"/>
+      <selection activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16.25" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="16.2" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="27.6640625" style="24" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.33203125" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" customWidth="1"/>
-    <col min="5" max="5" width="10.83203125" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.83203125" customWidth="1"/>
-    <col min="11" max="11" width="10.83203125" customWidth="1"/>
-    <col min="13" max="13" width="10.83203125" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" customWidth="1"/>
-    <col min="19" max="19" width="10.83203125" customWidth="1"/>
-    <col min="21" max="21" width="10.83203125" customWidth="1"/>
-    <col min="22" max="22" width="10.1640625" customWidth="1"/>
-    <col min="23" max="23" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="10.1640625" customWidth="1"/>
+    <col min="5" max="5" width="10.77734375" customWidth="1"/>
+    <col min="7" max="7" width="11.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.77734375" customWidth="1"/>
+    <col min="11" max="11" width="10.77734375" customWidth="1"/>
+    <col min="13" max="13" width="10.77734375" customWidth="1"/>
+    <col min="15" max="15" width="10.77734375" customWidth="1"/>
+    <col min="17" max="17" width="10.77734375" customWidth="1"/>
+    <col min="19" max="19" width="10.77734375" customWidth="1"/>
+    <col min="21" max="21" width="10.77734375" customWidth="1"/>
+    <col min="22" max="22" width="10.109375" customWidth="1"/>
+    <col min="23" max="23" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="11.44140625" bestFit="1" customWidth="1"/>
     <col min="27" max="28" width="10" customWidth="1"/>
-    <col min="29" max="29" width="11.1640625" customWidth="1"/>
-    <col min="33" max="33" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="11.44140625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B1" s="24" t="s">
         <v>51</v>
       </c>
-      <c r="C1" s="26">
+      <c r="C1" s="27">
         <v>1</v>
       </c>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26">
+      <c r="D1" s="27"/>
+      <c r="E1" s="27">
         <v>2</v>
       </c>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26">
+      <c r="F1" s="27"/>
+      <c r="G1" s="27">
         <v>3</v>
       </c>
-      <c r="H1" s="26"/>
-      <c r="I1" s="26">
+      <c r="H1" s="27"/>
+      <c r="I1" s="27">
         <v>4</v>
       </c>
-      <c r="J1" s="26"/>
-      <c r="K1" s="26">
+      <c r="J1" s="27"/>
+      <c r="K1" s="27">
         <v>5</v>
       </c>
-      <c r="L1" s="26"/>
-      <c r="M1" s="26">
+      <c r="L1" s="27"/>
+      <c r="M1" s="27">
         <v>6</v>
       </c>
-      <c r="N1" s="26"/>
-      <c r="O1" s="26">
+      <c r="N1" s="27"/>
+      <c r="O1" s="27">
         <v>7</v>
       </c>
-      <c r="P1" s="26"/>
-      <c r="Q1" s="26">
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27">
         <v>8</v>
       </c>
-      <c r="R1" s="26"/>
-      <c r="S1" s="26">
+      <c r="R1" s="27"/>
+      <c r="S1" s="27">
         <v>9</v>
       </c>
-      <c r="T1" s="26"/>
-      <c r="U1" s="26">
+      <c r="T1" s="27"/>
+      <c r="U1" s="27">
         <v>10</v>
       </c>
-      <c r="V1" s="26"/>
-      <c r="W1" s="26">
+      <c r="V1" s="27"/>
+      <c r="W1" s="27">
         <v>11</v>
       </c>
-      <c r="X1" s="26"/>
-      <c r="Y1" s="26">
+      <c r="X1" s="27"/>
+      <c r="Y1" s="27">
         <v>12</v>
       </c>
-      <c r="Z1" s="26"/>
-      <c r="AA1" s="26">
+      <c r="Z1" s="27"/>
+      <c r="AA1" s="27">
         <v>13</v>
       </c>
-      <c r="AB1" s="26"/>
-      <c r="AC1" s="26">
+      <c r="AB1" s="27"/>
+      <c r="AC1" s="27">
         <v>14</v>
       </c>
-      <c r="AD1" s="26"/>
-      <c r="AE1" s="26">
+      <c r="AD1" s="27"/>
+      <c r="AE1" s="27">
         <v>15</v>
       </c>
-      <c r="AF1" s="26"/>
-    </row>
-    <row r="2" spans="1:32" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AF1" s="27"/>
+    </row>
+    <row r="2" spans="1:32" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>45</v>
       </c>
@@ -1146,7 +1146,7 @@
       <c r="AE2" s="2"/>
       <c r="AF2" s="2"/>
     </row>
-    <row r="3" spans="1:32" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:32" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A3" s="24" t="s">
         <v>0</v>
       </c>
@@ -1226,7 +1226,7 @@
       <c r="AC3" s="3"/>
       <c r="AD3" s="3"/>
     </row>
-    <row r="4" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:32" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="24" t="s">
         <v>4</v>
       </c>
@@ -1286,7 +1286,7 @@
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
     </row>
-    <row r="5" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:32" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="24" t="s">
         <v>6</v>
       </c>
@@ -1358,7 +1358,7 @@
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
     </row>
-    <row r="6" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:32" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="24" t="s">
         <v>7</v>
       </c>
@@ -1412,7 +1412,7 @@
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
     </row>
-    <row r="7" spans="1:32" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="24" t="s">
         <v>98</v>
       </c>
@@ -1460,7 +1460,7 @@
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
     </row>
-    <row r="8" spans="1:32" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="1" t="s">
         <v>28</v>
       </c>
@@ -1490,7 +1490,7 @@
       <c r="AC8" s="2"/>
       <c r="AD8" s="4"/>
     </row>
-    <row r="9" spans="1:32" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:32" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A9" s="24" t="s">
         <v>9</v>
       </c>
@@ -1563,8 +1563,8 @@
       <c r="X9" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="Y9" s="27" t="s">
-        <v>117</v>
+      <c r="Y9" s="26" t="s">
+        <v>116</v>
       </c>
       <c r="Z9" t="s">
         <v>102</v>
@@ -1575,8 +1575,8 @@
       <c r="AB9" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AC9" s="27" t="s">
-        <v>117</v>
+      <c r="AC9" s="26" t="s">
+        <v>116</v>
       </c>
       <c r="AD9" t="s">
         <v>101</v>
@@ -1588,7 +1588,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:32" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="24" t="s">
         <v>10</v>
       </c>
@@ -1661,8 +1661,8 @@
       <c r="X10" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="Y10" s="27" t="s">
-        <v>117</v>
+      <c r="Y10" s="26" t="s">
+        <v>116</v>
       </c>
       <c r="Z10" t="s">
         <v>102</v>
@@ -1673,8 +1673,8 @@
       <c r="AB10" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="AC10" s="27" t="s">
-        <v>117</v>
+      <c r="AC10" s="26" t="s">
+        <v>116</v>
       </c>
       <c r="AD10" t="s">
         <v>101</v>
@@ -1686,7 +1686,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:32" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>113</v>
       </c>
@@ -1706,7 +1706,7 @@
         <v>67</v>
       </c>
       <c r="G11" s="25" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="H11" t="s">
         <v>115</v>
@@ -1760,7 +1760,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:32" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:32" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A12" s="1" t="s">
         <v>29</v>
       </c>
@@ -1793,7 +1793,7 @@
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
     </row>
-    <row r="13" spans="1:32" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:32" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A13" s="24" t="s">
         <v>30</v>
       </c>
@@ -1857,7 +1857,7 @@
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
     </row>
-    <row r="14" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:32" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="24" t="s">
         <v>31</v>
       </c>
@@ -1920,7 +1920,7 @@
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
     </row>
-    <row r="15" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:32" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="24" t="s">
         <v>33</v>
       </c>
@@ -1984,7 +1984,7 @@
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
     </row>
-    <row r="16" spans="1:32" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:32" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="24" t="s">
         <v>32</v>
       </c>
@@ -2044,7 +2044,7 @@
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
     </row>
-    <row r="17" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="24" t="s">
         <v>34</v>
       </c>
@@ -2101,7 +2101,7 @@
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
     </row>
-    <row r="18" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="24" t="s">
         <v>35</v>
       </c>
@@ -2161,7 +2161,7 @@
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
     </row>
-    <row r="19" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="24" t="s">
         <v>36</v>
       </c>
@@ -2221,7 +2221,7 @@
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
     </row>
-    <row r="20" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="24" t="s">
         <v>37</v>
       </c>
@@ -2273,7 +2273,7 @@
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
     </row>
-    <row r="21" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="24" t="s">
         <v>38</v>
       </c>
@@ -2329,7 +2329,7 @@
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
     </row>
-    <row r="22" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="24" t="s">
         <v>39</v>
       </c>
@@ -2385,7 +2385,7 @@
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
     </row>
-    <row r="23" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="24" t="s">
         <v>40</v>
       </c>
@@ -2449,7 +2449,7 @@
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
     </row>
-    <row r="24" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="24" t="s">
         <v>100</v>
       </c>
@@ -2505,7 +2505,7 @@
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
     </row>
-    <row r="25" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="24" t="s">
         <v>41</v>
       </c>
@@ -2555,7 +2555,7 @@
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
     </row>
-    <row r="26" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="24" t="s">
         <v>42</v>
       </c>
@@ -2611,7 +2611,7 @@
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
     </row>
-    <row r="27" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="24" t="s">
         <v>43</v>
       </c>
@@ -2659,7 +2659,7 @@
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
     </row>
-    <row r="28" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:30" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A28" s="24" t="s">
         <v>44</v>
       </c>
@@ -2707,12 +2707,12 @@
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
     </row>
-    <row r="29" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:30" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="1" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A30" s="24" t="s">
         <v>90</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
     </row>
-    <row r="31" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="24" t="s">
         <v>91</v>
       </c>
@@ -2836,7 +2836,7 @@
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
     </row>
-    <row r="32" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A32" s="24" t="s">
         <v>92</v>
       </c>
@@ -2892,7 +2892,7 @@
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
     </row>
-    <row r="33" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="24" t="s">
         <v>93</v>
       </c>
@@ -2940,7 +2940,7 @@
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
     </row>
-    <row r="34" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A34" s="24" t="s">
         <v>94</v>
       </c>
@@ -2996,7 +2996,7 @@
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
     </row>
-    <row r="35" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A35" s="24" t="s">
         <v>95</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
     </row>
-    <row r="36" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="24" t="s">
         <v>96</v>
       </c>
@@ -3098,7 +3098,7 @@
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
     </row>
-    <row r="37" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:30" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A37" s="24" t="s">
         <v>97</v>
       </c>
@@ -3150,7 +3150,7 @@
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
     </row>
-    <row r="38" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:30" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A38" s="1" t="s">
         <v>24</v>
       </c>
@@ -3181,7 +3181,7 @@
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
     </row>
-    <row r="39" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A39" s="24" t="s">
         <v>23</v>
       </c>
@@ -3263,7 +3263,7 @@
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
     </row>
-    <row r="40" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="24" t="s">
         <v>23</v>
       </c>
@@ -3345,7 +3345,7 @@
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
     </row>
-    <row r="41" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A41" s="24" t="s">
         <v>23</v>
       </c>
@@ -3427,7 +3427,7 @@
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
     </row>
-    <row r="42" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="24" t="s">
         <v>23</v>
       </c>
@@ -3509,7 +3509,7 @@
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
     </row>
-    <row r="43" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A43" s="24" t="s">
         <v>23</v>
       </c>
@@ -3591,7 +3591,7 @@
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
     </row>
-    <row r="44" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A44" s="24" t="s">
         <v>23</v>
       </c>
@@ -3673,7 +3673,7 @@
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
     </row>
-    <row r="45" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="24" t="s">
         <v>23</v>
       </c>
@@ -3755,7 +3755,7 @@
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
     </row>
-    <row r="46" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="24" t="s">
         <v>46</v>
       </c>
@@ -3837,7 +3837,7 @@
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
     </row>
-    <row r="47" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A47" s="24" t="s">
         <v>46</v>
       </c>
@@ -3921,7 +3921,7 @@
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
     </row>
-    <row r="48" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A48" s="24" t="s">
         <v>46</v>
       </c>
@@ -4005,7 +4005,7 @@
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
     </row>
-    <row r="49" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A49" s="24" t="s">
         <v>46</v>
       </c>
@@ -4089,7 +4089,7 @@
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
     </row>
-    <row r="50" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A50" s="24" t="s">
         <v>47</v>
       </c>
@@ -4173,7 +4173,7 @@
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
     </row>
-    <row r="51" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A51" s="24" t="s">
         <v>47</v>
       </c>
@@ -4257,7 +4257,7 @@
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
     </row>
-    <row r="52" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A52" s="24" t="s">
         <v>47</v>
       </c>
@@ -4341,7 +4341,7 @@
       <c r="AC52" s="3"/>
       <c r="AD52" s="3"/>
     </row>
-    <row r="53" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53" s="24" t="s">
         <v>47</v>
       </c>
@@ -4425,7 +4425,7 @@
       <c r="AC53" s="3"/>
       <c r="AD53" s="3"/>
     </row>
-    <row r="54" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A54" s="24" t="s">
         <v>47</v>
       </c>
@@ -4509,7 +4509,7 @@
       <c r="AC54" s="3"/>
       <c r="AD54" s="3"/>
     </row>
-    <row r="55" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A55" s="24" t="s">
         <v>47</v>
       </c>
@@ -4593,7 +4593,7 @@
       <c r="AC55" s="3"/>
       <c r="AD55" s="3"/>
     </row>
-    <row r="56" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A56" s="24" t="s">
         <v>47</v>
       </c>
@@ -4677,7 +4677,7 @@
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
     </row>
-    <row r="57" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A57" s="24" t="s">
         <v>48</v>
       </c>
@@ -4761,7 +4761,7 @@
       <c r="AC57" s="3"/>
       <c r="AD57" s="3"/>
     </row>
-    <row r="58" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A58" s="24" t="s">
         <v>48</v>
       </c>
@@ -4845,7 +4845,7 @@
       <c r="AC58" s="3"/>
       <c r="AD58" s="3"/>
     </row>
-    <row r="59" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A59" s="24" t="s">
         <v>48</v>
       </c>
@@ -4929,7 +4929,7 @@
       <c r="AC59" s="3"/>
       <c r="AD59" s="3"/>
     </row>
-    <row r="60" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A60" s="24" t="s">
         <v>48</v>
       </c>
@@ -5013,7 +5013,7 @@
       <c r="AC60" s="3"/>
       <c r="AD60" s="3"/>
     </row>
-    <row r="61" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A61" s="24" t="s">
         <v>49</v>
       </c>
@@ -5073,7 +5073,7 @@
       <c r="AC61" s="3"/>
       <c r="AD61" s="3"/>
     </row>
-    <row r="62" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A62" s="24" t="s">
         <v>49</v>
       </c>
@@ -5133,7 +5133,7 @@
       <c r="AC62" s="3"/>
       <c r="AD62" s="3"/>
     </row>
-    <row r="63" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A63" s="24" t="s">
         <v>49</v>
       </c>
@@ -5193,7 +5193,7 @@
       <c r="AC63" s="3"/>
       <c r="AD63" s="3"/>
     </row>
-    <row r="64" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:30" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="24" t="s">
         <v>8</v>
       </c>
@@ -5253,7 +5253,7 @@
       <c r="AC64" s="3"/>
       <c r="AD64" s="3"/>
     </row>
-    <row r="65" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:30" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A65" s="1" t="s">
         <v>25</v>
       </c>
@@ -5287,7 +5287,7 @@
       <c r="AC65" s="3"/>
       <c r="AD65" s="3"/>
     </row>
-    <row r="66" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:30" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A66" s="24" t="s">
         <v>20</v>
       </c>
@@ -5355,7 +5355,7 @@
       <c r="AC66" s="3"/>
       <c r="AD66" s="3"/>
     </row>
-    <row r="67" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A67" s="24" t="s">
         <v>20</v>
       </c>
@@ -5423,7 +5423,7 @@
       <c r="AC67" s="3"/>
       <c r="AD67" s="3"/>
     </row>
-    <row r="68" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A68" s="24" t="s">
         <v>20</v>
       </c>
@@ -5491,7 +5491,7 @@
       <c r="AC68" s="3"/>
       <c r="AD68" s="3"/>
     </row>
-    <row r="69" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A69" s="24" t="s">
         <v>20</v>
       </c>
@@ -5561,7 +5561,7 @@
       <c r="AC69" s="3"/>
       <c r="AD69" s="3"/>
     </row>
-    <row r="70" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A70" s="24" t="s">
         <v>21</v>
       </c>
@@ -5637,7 +5637,7 @@
       <c r="AC70" s="3"/>
       <c r="AD70" s="3"/>
     </row>
-    <row r="71" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A71" s="24" t="s">
         <v>21</v>
       </c>
@@ -5713,7 +5713,7 @@
       <c r="AC71" s="3"/>
       <c r="AD71" s="3"/>
     </row>
-    <row r="72" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A72" s="24" t="s">
         <v>21</v>
       </c>
@@ -5787,7 +5787,7 @@
       <c r="AC72" s="3"/>
       <c r="AD72" s="3"/>
     </row>
-    <row r="73" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A73" s="24" t="s">
         <v>21</v>
       </c>
@@ -5861,7 +5861,7 @@
       <c r="AC73" s="3"/>
       <c r="AD73" s="3"/>
     </row>
-    <row r="74" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A74" s="24" t="s">
         <v>22</v>
       </c>
@@ -5919,7 +5919,7 @@
       <c r="AC74" s="3"/>
       <c r="AD74" s="3"/>
     </row>
-    <row r="75" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:30" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A75" s="24" t="s">
         <v>22</v>
       </c>
@@ -5977,7 +5977,7 @@
       <c r="AC75" s="3"/>
       <c r="AD75" s="3"/>
     </row>
-    <row r="76" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:30" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A76" s="1" t="s">
         <v>27</v>
       </c>
@@ -6005,7 +6005,7 @@
       <c r="X76" s="4"/>
       <c r="Y76" s="4"/>
     </row>
-    <row r="77" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:30" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A77" s="24" t="s">
         <v>1</v>
       </c>
@@ -6068,7 +6068,7 @@
       <c r="X77" s="4"/>
       <c r="Y77" s="4"/>
     </row>
-    <row r="78" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A78" s="24" t="s">
         <v>1</v>
       </c>
@@ -6130,7 +6130,7 @@
       <c r="X78" s="4"/>
       <c r="Y78" s="4"/>
     </row>
-    <row r="79" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A79" s="24" t="s">
         <v>1</v>
       </c>
@@ -6193,7 +6193,7 @@
       <c r="X79" s="4"/>
       <c r="Y79" s="4"/>
     </row>
-    <row r="80" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A80" s="24" t="s">
         <v>1</v>
       </c>
@@ -6256,7 +6256,7 @@
       <c r="X80" s="4"/>
       <c r="Y80" s="4"/>
     </row>
-    <row r="81" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A81" s="24" t="s">
         <v>88</v>
       </c>
@@ -6311,7 +6311,7 @@
       <c r="X81" s="4"/>
       <c r="Y81" s="4"/>
     </row>
-    <row r="82" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A82" s="24" t="s">
         <v>88</v>
       </c>
@@ -6366,7 +6366,7 @@
       <c r="X82" s="4"/>
       <c r="Y82" s="4"/>
     </row>
-    <row r="83" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A83" s="24" t="s">
         <v>2</v>
       </c>
@@ -6452,7 +6452,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="84" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A84" s="24" t="s">
         <v>2</v>
       </c>
@@ -6538,7 +6538,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="85" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A85" s="24" t="s">
         <v>2</v>
       </c>
@@ -6624,7 +6624,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="86" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A86" s="24" t="s">
         <v>2</v>
       </c>
@@ -6710,7 +6710,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="87" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A87" s="24" t="s">
         <v>2</v>
       </c>
@@ -6796,7 +6796,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="88" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A88" s="24" t="s">
         <v>2</v>
       </c>
@@ -6882,7 +6882,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="89" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A89" s="24" t="s">
         <v>2</v>
       </c>
@@ -6968,7 +6968,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="90" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A90" s="24" t="s">
         <v>2</v>
       </c>
@@ -7054,7 +7054,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A91" s="24" t="s">
         <v>3</v>
       </c>
@@ -7140,7 +7140,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="92" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A92" s="24" t="s">
         <v>3</v>
       </c>
@@ -7228,7 +7228,7 @@
       <c r="AC92" s="3"/>
       <c r="AD92" s="3"/>
     </row>
-    <row r="93" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A93" s="24" t="s">
         <v>3</v>
       </c>
@@ -7316,7 +7316,7 @@
       <c r="AC93" s="3"/>
       <c r="AD93" s="3"/>
     </row>
-    <row r="94" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A94" s="24" t="s">
         <v>3</v>
       </c>
@@ -7404,7 +7404,7 @@
       <c r="AC94" s="3"/>
       <c r="AD94" s="3"/>
     </row>
-    <row r="95" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A95" s="24" t="s">
         <v>3</v>
       </c>
@@ -7492,7 +7492,7 @@
       <c r="AC95" s="3"/>
       <c r="AD95" s="3"/>
     </row>
-    <row r="96" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A96" s="24" t="s">
         <v>3</v>
       </c>
@@ -7580,7 +7580,7 @@
       <c r="AC96" s="3"/>
       <c r="AD96" s="3"/>
     </row>
-    <row r="97" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A97" s="24" t="s">
         <v>3</v>
       </c>
@@ -7668,7 +7668,7 @@
       <c r="AC97" s="3"/>
       <c r="AD97" s="3"/>
     </row>
-    <row r="98" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A98" s="24" t="s">
         <v>55</v>
       </c>
@@ -7736,7 +7736,7 @@
       <c r="AC98" s="3"/>
       <c r="AD98" s="3"/>
     </row>
-    <row r="99" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A99" s="24" t="s">
         <v>55</v>
       </c>
@@ -7801,7 +7801,7 @@
       <c r="AC99" s="3"/>
       <c r="AD99" s="3"/>
     </row>
-    <row r="100" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A100" s="24" t="s">
         <v>55</v>
       </c>
@@ -7866,7 +7866,7 @@
       <c r="AC100" s="3"/>
       <c r="AD100" s="3"/>
     </row>
-    <row r="101" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A101" s="24" t="s">
         <v>55</v>
       </c>
@@ -7931,7 +7931,7 @@
       <c r="AC101" s="3"/>
       <c r="AD101" s="3"/>
     </row>
-    <row r="102" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A102" s="24" t="s">
         <v>11</v>
       </c>
@@ -8000,7 +8000,7 @@
       <c r="AC102" s="3"/>
       <c r="AD102" s="3"/>
     </row>
-    <row r="103" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A103" s="24" t="s">
         <v>11</v>
       </c>
@@ -8069,7 +8069,7 @@
       <c r="AC103" s="3"/>
       <c r="AD103" s="3"/>
     </row>
-    <row r="104" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A104" s="24" t="s">
         <v>11</v>
       </c>
@@ -8138,7 +8138,7 @@
       <c r="AC104" s="3"/>
       <c r="AD104" s="3"/>
     </row>
-    <row r="105" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A105" s="24" t="s">
         <v>11</v>
       </c>
@@ -8207,7 +8207,7 @@
       <c r="AC105" s="3"/>
       <c r="AD105" s="3"/>
     </row>
-    <row r="106" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A106" s="24" t="s">
         <v>11</v>
       </c>
@@ -8276,7 +8276,7 @@
       <c r="AC106" s="3"/>
       <c r="AD106" s="3"/>
     </row>
-    <row r="107" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A107" s="24" t="s">
         <v>5</v>
       </c>
@@ -8341,7 +8341,7 @@
       <c r="AC107" s="3"/>
       <c r="AD107" s="3"/>
     </row>
-    <row r="108" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A108" s="24" t="s">
         <v>5</v>
       </c>
@@ -8406,7 +8406,7 @@
       <c r="AC108" s="3"/>
       <c r="AD108" s="3"/>
     </row>
-    <row r="109" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A109" s="24" t="s">
         <v>5</v>
       </c>
@@ -8471,7 +8471,7 @@
       <c r="AC109" s="3"/>
       <c r="AD109" s="3"/>
     </row>
-    <row r="110" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A110" s="24" t="s">
         <v>5</v>
       </c>
@@ -8536,7 +8536,7 @@
       <c r="AC110" s="3"/>
       <c r="AD110" s="3"/>
     </row>
-    <row r="111" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A111" s="24" t="s">
         <v>12</v>
       </c>
@@ -8585,7 +8585,7 @@
       <c r="AC111" s="3"/>
       <c r="AD111" s="3"/>
     </row>
-    <row r="112" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A112" s="24" t="s">
         <v>12</v>
       </c>
@@ -8634,7 +8634,7 @@
       <c r="AC112" s="3"/>
       <c r="AD112" s="3"/>
     </row>
-    <row r="113" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A113" s="24" t="s">
         <v>12</v>
       </c>
@@ -8683,7 +8683,7 @@
       <c r="AC113" s="3"/>
       <c r="AD113" s="3"/>
     </row>
-    <row r="114" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A114" s="24" t="s">
         <v>12</v>
       </c>
@@ -8735,7 +8735,7 @@
       <c r="AC114" s="3"/>
       <c r="AD114" s="3"/>
     </row>
-    <row r="115" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A115" s="24" t="s">
         <v>13</v>
       </c>
@@ -8783,7 +8783,7 @@
       <c r="AC115" s="3"/>
       <c r="AD115" s="3"/>
     </row>
-    <row r="116" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A116" s="24" t="s">
         <v>13</v>
       </c>
@@ -8831,7 +8831,7 @@
       <c r="AC116" s="3"/>
       <c r="AD116" s="3"/>
     </row>
-    <row r="117" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A117" s="24" t="s">
         <v>112</v>
       </c>
@@ -8873,7 +8873,7 @@
       <c r="AC117" s="3"/>
       <c r="AD117" s="3"/>
     </row>
-    <row r="118" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A118" s="24" t="s">
         <v>103</v>
       </c>
@@ -8953,7 +8953,7 @@
       <c r="AC118" s="3"/>
       <c r="AD118" s="3"/>
     </row>
-    <row r="119" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A119" s="24" t="s">
         <v>104</v>
       </c>
@@ -9033,7 +9033,7 @@
       <c r="AC119" s="3"/>
       <c r="AD119" s="3"/>
     </row>
-    <row r="120" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A120" s="24" t="s">
         <v>105</v>
       </c>
@@ -9113,7 +9113,7 @@
       <c r="AC120" s="3"/>
       <c r="AD120" s="3"/>
     </row>
-    <row r="121" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A121" s="24" t="s">
         <v>106</v>
       </c>
@@ -9193,7 +9193,7 @@
       <c r="AC121" s="3"/>
       <c r="AD121" s="3"/>
     </row>
-    <row r="122" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A122" s="24" t="s">
         <v>107</v>
       </c>
@@ -9273,7 +9273,7 @@
       <c r="AC122" s="3"/>
       <c r="AD122" s="3"/>
     </row>
-    <row r="123" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A123" s="24" t="s">
         <v>108</v>
       </c>
@@ -9353,7 +9353,7 @@
       <c r="AC123" s="3"/>
       <c r="AD123" s="3"/>
     </row>
-    <row r="124" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A124" s="24" t="s">
         <v>109</v>
       </c>
@@ -9433,7 +9433,7 @@
       <c r="AC124" s="3"/>
       <c r="AD124" s="3"/>
     </row>
-    <row r="125" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A125" s="24" t="s">
         <v>110</v>
       </c>
@@ -9513,7 +9513,7 @@
       <c r="AC125" s="3"/>
       <c r="AD125" s="3"/>
     </row>
-    <row r="126" spans="1:30" ht="16.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:30" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A126" s="24" t="s">
         <v>111</v>
       </c>
@@ -9593,7 +9593,7 @@
       <c r="AC126" s="3"/>
       <c r="AD126" s="3"/>
     </row>
-    <row r="127" spans="1:30" ht="16.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:30" ht="16.2" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A127" s="1" t="s">
         <v>26</v>
       </c>
@@ -9626,7 +9626,7 @@
       <c r="AC127" s="3"/>
       <c r="AD127" s="3"/>
     </row>
-    <row r="128" spans="1:30" ht="16.25" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:30" ht="16.2" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A128" s="24" t="s">
         <v>14</v>
       </c>
@@ -9678,7 +9678,7 @@
       <c r="AC128" s="3"/>
       <c r="AD128" s="3"/>
     </row>
-    <row r="129" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A129" s="24" t="s">
         <v>14</v>
       </c>
@@ -9730,7 +9730,7 @@
       <c r="AC129" s="3"/>
       <c r="AD129" s="3"/>
     </row>
-    <row r="130" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A130" s="24" t="s">
         <v>14</v>
       </c>
@@ -9782,7 +9782,7 @@
       <c r="AC130" s="3"/>
       <c r="AD130" s="3"/>
     </row>
-    <row r="131" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A131" s="24" t="s">
         <v>14</v>
       </c>
@@ -9834,7 +9834,7 @@
       <c r="AC131" s="3"/>
       <c r="AD131" s="3"/>
     </row>
-    <row r="132" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A132" s="24" t="s">
         <v>14</v>
       </c>
@@ -9886,7 +9886,7 @@
       <c r="AC132" s="3"/>
       <c r="AD132" s="3"/>
     </row>
-    <row r="133" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A133" s="24" t="s">
         <v>15</v>
       </c>
@@ -9946,7 +9946,7 @@
       <c r="AC133" s="3"/>
       <c r="AD133" s="3"/>
     </row>
-    <row r="134" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A134" s="24" t="s">
         <v>15</v>
       </c>
@@ -10006,7 +10006,7 @@
       <c r="AC134" s="3"/>
       <c r="AD134" s="3"/>
     </row>
-    <row r="135" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A135" s="24" t="s">
         <v>15</v>
       </c>
@@ -10066,7 +10066,7 @@
       <c r="AC135" s="3"/>
       <c r="AD135" s="3"/>
     </row>
-    <row r="136" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A136" s="24" t="s">
         <v>15</v>
       </c>
@@ -10126,7 +10126,7 @@
       <c r="AC136" s="3"/>
       <c r="AD136" s="3"/>
     </row>
-    <row r="137" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A137" s="24" t="s">
         <v>15</v>
       </c>
@@ -10186,7 +10186,7 @@
       <c r="AC137" s="3"/>
       <c r="AD137" s="3"/>
     </row>
-    <row r="138" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A138" s="24" t="s">
         <v>15</v>
       </c>
@@ -10246,7 +10246,7 @@
       <c r="AC138" s="3"/>
       <c r="AD138" s="3"/>
     </row>
-    <row r="139" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A139" s="24" t="s">
         <v>16</v>
       </c>
@@ -10298,7 +10298,7 @@
       <c r="AC139" s="3"/>
       <c r="AD139" s="3"/>
     </row>
-    <row r="140" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A140" s="24" t="s">
         <v>16</v>
       </c>
@@ -10350,7 +10350,7 @@
       <c r="AC140" s="3"/>
       <c r="AD140" s="3"/>
     </row>
-    <row r="141" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A141" s="24" t="s">
         <v>16</v>
       </c>
@@ -10402,7 +10402,7 @@
       <c r="AC141" s="3"/>
       <c r="AD141" s="3"/>
     </row>
-    <row r="142" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A142" s="24" t="s">
         <v>16</v>
       </c>
@@ -10454,7 +10454,7 @@
       <c r="AC142" s="3"/>
       <c r="AD142" s="3"/>
     </row>
-    <row r="143" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A143" s="24" t="s">
         <v>16</v>
       </c>
@@ -10506,7 +10506,7 @@
       <c r="AC143" s="3"/>
       <c r="AD143" s="3"/>
     </row>
-    <row r="144" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A144" s="24" t="s">
         <v>17</v>
       </c>
@@ -10554,7 +10554,7 @@
       <c r="AC144" s="3"/>
       <c r="AD144" s="3"/>
     </row>
-    <row r="145" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A145" s="24" t="s">
         <v>17</v>
       </c>
@@ -10602,7 +10602,7 @@
       <c r="AC145" s="3"/>
       <c r="AD145" s="3"/>
     </row>
-    <row r="146" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A146" s="24" t="s">
         <v>17</v>
       </c>
@@ -10650,7 +10650,7 @@
       <c r="AC146" s="3"/>
       <c r="AD146" s="3"/>
     </row>
-    <row r="147" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A147" s="24" t="s">
         <v>17</v>
       </c>
@@ -10698,7 +10698,7 @@
       <c r="AC147" s="3"/>
       <c r="AD147" s="3"/>
     </row>
-    <row r="148" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A148" s="24" t="s">
         <v>17</v>
       </c>
@@ -10746,7 +10746,7 @@
       <c r="AC148" s="3"/>
       <c r="AD148" s="3"/>
     </row>
-    <row r="149" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A149" s="24" t="s">
         <v>18</v>
       </c>
@@ -10794,7 +10794,7 @@
       <c r="AC149" s="3"/>
       <c r="AD149" s="3"/>
     </row>
-    <row r="150" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A150" s="24" t="s">
         <v>18</v>
       </c>
@@ -10842,7 +10842,7 @@
       <c r="AC150" s="3"/>
       <c r="AD150" s="3"/>
     </row>
-    <row r="151" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A151" s="24" t="s">
         <v>18</v>
       </c>
@@ -10890,7 +10890,7 @@
       <c r="AC151" s="3"/>
       <c r="AD151" s="3"/>
     </row>
-    <row r="152" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A152" s="24" t="s">
         <v>19</v>
       </c>
@@ -10930,7 +10930,7 @@
       <c r="AC152" s="3"/>
       <c r="AD152" s="3"/>
     </row>
-    <row r="153" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A153" s="24" t="s">
         <v>19</v>
       </c>
@@ -10970,7 +10970,7 @@
       <c r="AC153" s="3"/>
       <c r="AD153" s="3"/>
     </row>
-    <row r="154" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A154" s="24" t="s">
         <v>19</v>
       </c>
@@ -11010,7 +11010,7 @@
       <c r="AC154" s="3"/>
       <c r="AD154" s="3"/>
     </row>
-    <row r="155" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A155" s="24" t="s">
         <v>19</v>
       </c>
@@ -11050,7 +11050,7 @@
       <c r="AC155" s="3"/>
       <c r="AD155" s="3"/>
     </row>
-    <row r="156" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A156" s="24" t="s">
         <v>19</v>
       </c>
@@ -11090,7 +11090,7 @@
       <c r="AC156" s="3"/>
       <c r="AD156" s="3"/>
     </row>
-    <row r="157" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A157" s="24" t="s">
         <v>19</v>
       </c>
@@ -11130,7 +11130,7 @@
       <c r="AC157" s="3"/>
       <c r="AD157" s="3"/>
     </row>
-    <row r="158" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="C158" s="4"/>
       <c r="D158" s="4"/>
       <c r="E158" s="4"/>
@@ -11160,119 +11160,119 @@
       <c r="AC158" s="3"/>
       <c r="AD158" s="3"/>
     </row>
-    <row r="159" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z159" s="4"/>
       <c r="AA159" s="4"/>
       <c r="AB159" s="4"/>
       <c r="AC159" s="3"/>
       <c r="AD159" s="3"/>
     </row>
-    <row r="160" spans="1:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z160" s="4"/>
       <c r="AA160" s="4"/>
       <c r="AB160" s="4"/>
       <c r="AC160" s="3"/>
       <c r="AD160" s="3"/>
     </row>
-    <row r="161" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="161" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z161" s="4"/>
       <c r="AA161" s="4"/>
       <c r="AB161" s="4"/>
       <c r="AC161" s="3"/>
       <c r="AD161" s="3"/>
     </row>
-    <row r="162" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="162" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z162" s="4"/>
       <c r="AA162" s="4"/>
       <c r="AB162" s="4"/>
       <c r="AC162" s="3"/>
       <c r="AD162" s="3"/>
     </row>
-    <row r="163" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="163" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z163" s="4"/>
       <c r="AA163" s="4"/>
       <c r="AB163" s="4"/>
       <c r="AC163" s="3"/>
       <c r="AD163" s="3"/>
     </row>
-    <row r="164" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="164" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z164" s="4"/>
       <c r="AA164" s="4"/>
       <c r="AB164" s="4"/>
       <c r="AC164" s="3"/>
       <c r="AD164" s="3"/>
     </row>
-    <row r="165" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="165" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z165" s="4"/>
       <c r="AA165" s="4"/>
       <c r="AB165" s="4"/>
       <c r="AC165" s="3"/>
       <c r="AD165" s="3"/>
     </row>
-    <row r="166" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="166" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z166" s="4"/>
       <c r="AA166" s="4"/>
       <c r="AB166" s="4"/>
       <c r="AC166" s="3"/>
       <c r="AD166" s="3"/>
     </row>
-    <row r="167" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="167" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z167" s="4"/>
       <c r="AA167" s="4"/>
       <c r="AB167" s="4"/>
       <c r="AC167" s="3"/>
       <c r="AD167" s="3"/>
     </row>
-    <row r="168" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="168" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z168" s="4"/>
       <c r="AA168" s="4"/>
       <c r="AB168" s="4"/>
       <c r="AC168" s="3"/>
       <c r="AD168" s="3"/>
     </row>
-    <row r="169" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="169" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z169" s="4"/>
       <c r="AA169" s="4"/>
       <c r="AB169" s="4"/>
       <c r="AC169" s="3"/>
       <c r="AD169" s="3"/>
     </row>
-    <row r="170" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="170" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z170" s="4"/>
       <c r="AA170" s="4"/>
       <c r="AB170" s="4"/>
       <c r="AC170" s="3"/>
       <c r="AD170" s="3"/>
     </row>
-    <row r="171" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="171" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z171" s="4"/>
       <c r="AA171" s="4"/>
       <c r="AB171" s="4"/>
       <c r="AC171" s="3"/>
       <c r="AD171" s="3"/>
     </row>
-    <row r="172" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="172" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z172" s="4"/>
       <c r="AA172" s="4"/>
       <c r="AB172" s="4"/>
       <c r="AC172" s="3"/>
       <c r="AD172" s="3"/>
     </row>
-    <row r="173" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="173" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z173" s="4"/>
       <c r="AA173" s="4"/>
       <c r="AB173" s="4"/>
       <c r="AC173" s="3"/>
       <c r="AD173" s="3"/>
     </row>
-    <row r="174" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="174" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="Z174" s="4"/>
       <c r="AA174" s="4"/>
       <c r="AB174" s="4"/>
       <c r="AC174" s="3"/>
       <c r="AD174" s="3"/>
     </row>
-    <row r="175" spans="26:30" ht="16.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="175" spans="26:30" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="AA175" s="4"/>
       <c r="AB175" s="4"/>
       <c r="AC175" s="3"/>

</xml_diff>